<commit_message>
wip: renamed external_id to ref_number added validation for uniqueness for firms and events
</commit_message>
<xml_diff>
--- a/graphql/db/events.xlsx
+++ b/graphql/db/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D8E932-2AF9-F049-A843-BDBF57A316B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6C473F-502E-D445-A84C-D6B171E25EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8580" yWindow="1420" windowWidth="28380" windowHeight="18980" xr2:uid="{E724A02B-0613-6046-AB06-036B70DCFCC0}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>duration_time</t>
   </si>
   <si>
-    <t>external_id</t>
-  </si>
-  <si>
     <t>max_attendees</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>firm_ref</t>
+  </si>
+  <si>
+    <t>ref_number</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,7 +683,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -707,22 +707,22 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>8</v>
@@ -730,16 +730,16 @@
     </row>
     <row r="2" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1">
         <v>32500</v>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2" s="1">
         <v>10</v>
@@ -766,24 +766,24 @@
         <v>45137</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1">
         <v>43500</v>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="1">
         <v>10</v>
@@ -807,24 +807,24 @@
         <v>4</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1">
         <v>12500</v>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J4" s="1">
         <v>10</v>
@@ -848,24 +848,24 @@
         <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1">
         <v>34000</v>
@@ -880,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5" s="1">
         <v>10</v>
@@ -889,24 +889,24 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1">
         <v>9000</v>
@@ -921,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J6" s="1">
         <v>10</v>
@@ -930,24 +930,24 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1">
         <v>12500</v>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J7" s="1">
         <v>10</v>
@@ -971,24 +971,24 @@
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1">
         <v>75000</v>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J8" s="1">
         <v>10</v>
@@ -1015,24 +1015,24 @@
         <v>45168</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1">
         <v>30000</v>
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="1">
         <v>10</v>
@@ -1056,24 +1056,24 @@
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1">
         <v>10000</v>
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" s="1">
         <v>10</v>
@@ -1097,24 +1097,24 @@
         <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1">
         <v>12000</v>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J11" s="1">
         <v>10</v>
@@ -1138,24 +1138,24 @@
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1">
         <v>5000</v>
@@ -1170,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J12" s="1">
         <v>10</v>
@@ -1182,24 +1182,24 @@
         <v>45122</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1">
         <v>9500</v>
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="1">
         <v>10</v>
@@ -1223,24 +1223,24 @@
         <v>0</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E14" s="1">
         <v>12000</v>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J14" s="1">
         <v>10</v>
@@ -1267,21 +1267,21 @@
         <v>45198.875</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1">
         <v>55000</v>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" s="1">
         <v>10</v>
@@ -1305,24 +1305,24 @@
         <v>4</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1">
         <v>10000</v>
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J16" s="1">
         <v>10</v>
@@ -1346,24 +1346,24 @@
         <v>0</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E17" s="1">
         <v>9000</v>
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17" s="1">
         <v>10</v>
@@ -1390,27 +1390,27 @@
         <v>45199</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N17" s="4">
         <v>45198.875</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1">
         <v>13000</v>
@@ -1425,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
@@ -1434,24 +1434,24 @@
         <v>0</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1">
         <v>9000</v>
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J19" s="1">
         <v>10</v>
@@ -1475,24 +1475,24 @@
         <v>0</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E20" s="1">
         <v>30000</v>
@@ -1507,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="1">
         <v>10</v>
@@ -1516,24 +1516,24 @@
         <v>0</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="1">
         <v>10000</v>
@@ -1548,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J21" s="1">
         <v>10</v>
@@ -1557,10 +1557,10 @@
         <v>0</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: improved events table (#162)
* wip: improved events table

* wip: added bookings table

* wip: unified schedules

* wip: refactored headers and columns usage

* wip: added publish/unpublish event

* wip: added removed button

* wip: addedc reschedule functionality

* wip: renamed external_id to ref_number
added validation for uniqueness for firms and events

* wip: fixed tests

* wip: impoved alignment cells for table

* wip: added attendee options

* wip: small improvements

* wip: fixed rspec
</commit_message>
<xml_diff>
--- a/graphql/db/events.xlsx
+++ b/graphql/db/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D8E932-2AF9-F049-A843-BDBF57A316B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6C473F-502E-D445-A84C-D6B171E25EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8580" yWindow="1420" windowWidth="28380" windowHeight="18980" xr2:uid="{E724A02B-0613-6046-AB06-036B70DCFCC0}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>duration_time</t>
   </si>
   <si>
-    <t>external_id</t>
-  </si>
-  <si>
     <t>max_attendees</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>firm_ref</t>
+  </si>
+  <si>
+    <t>ref_number</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,7 +683,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -707,22 +707,22 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>8</v>
@@ -730,16 +730,16 @@
     </row>
     <row r="2" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1">
         <v>32500</v>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2" s="1">
         <v>10</v>
@@ -766,24 +766,24 @@
         <v>45137</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1">
         <v>43500</v>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="1">
         <v>10</v>
@@ -807,24 +807,24 @@
         <v>4</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1">
         <v>12500</v>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J4" s="1">
         <v>10</v>
@@ -848,24 +848,24 @@
         <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1">
         <v>34000</v>
@@ -880,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5" s="1">
         <v>10</v>
@@ -889,24 +889,24 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1">
         <v>9000</v>
@@ -921,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J6" s="1">
         <v>10</v>
@@ -930,24 +930,24 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1">
         <v>12500</v>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J7" s="1">
         <v>10</v>
@@ -971,24 +971,24 @@
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1">
         <v>75000</v>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J8" s="1">
         <v>10</v>
@@ -1015,24 +1015,24 @@
         <v>45168</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1">
         <v>30000</v>
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="1">
         <v>10</v>
@@ -1056,24 +1056,24 @@
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1">
         <v>10000</v>
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J10" s="1">
         <v>10</v>
@@ -1097,24 +1097,24 @@
         <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1">
         <v>12000</v>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J11" s="1">
         <v>10</v>
@@ -1138,24 +1138,24 @@
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1">
         <v>5000</v>
@@ -1170,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J12" s="1">
         <v>10</v>
@@ -1182,24 +1182,24 @@
         <v>45122</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1">
         <v>9500</v>
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="1">
         <v>10</v>
@@ -1223,24 +1223,24 @@
         <v>0</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E14" s="1">
         <v>12000</v>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J14" s="1">
         <v>10</v>
@@ -1267,21 +1267,21 @@
         <v>45198.875</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1">
         <v>55000</v>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" s="1">
         <v>10</v>
@@ -1305,24 +1305,24 @@
         <v>4</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1">
         <v>10000</v>
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J16" s="1">
         <v>10</v>
@@ -1346,24 +1346,24 @@
         <v>0</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E17" s="1">
         <v>9000</v>
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J17" s="1">
         <v>10</v>
@@ -1390,27 +1390,27 @@
         <v>45199</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N17" s="4">
         <v>45198.875</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1">
         <v>13000</v>
@@ -1425,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
@@ -1434,24 +1434,24 @@
         <v>0</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1">
         <v>9000</v>
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J19" s="1">
         <v>10</v>
@@ -1475,24 +1475,24 @@
         <v>0</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E20" s="1">
         <v>30000</v>
@@ -1507,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="1">
         <v>10</v>
@@ -1516,24 +1516,24 @@
         <v>0</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="1">
         <v>10000</v>
@@ -1548,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J21" s="1">
         <v>10</v>
@@ -1557,10 +1557,10 @@
         <v>0</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: changed seed for events
</commit_message>
<xml_diff>
--- a/graphql/db/events.xlsx
+++ b/graphql/db/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A74905-64BF-1D4A-92B8-1B3181524669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F9CDA6-F72C-1941-A338-54A2313A703F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="4240" windowWidth="36880" windowHeight="23500" xr2:uid="{E724A02B-0613-6046-AB06-036B70DCFCC0}"/>
+    <workbookView xWindow="12220" yWindow="5840" windowWidth="36880" windowHeight="23500" xr2:uid="{E724A02B-0613-6046-AB06-036B70DCFCC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE1BE4E-41DA-D14E-BD6A-74D507CD06A8}">
   <dimension ref="A1:O363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
-      <selection activeCell="D363" sqref="D363"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">RANDBETWEEN(10000, 999999999)</f>
-        <v>625331540</v>
+        <v>121775653</v>
       </c>
       <c r="J2" s="1">
         <v>10</v>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I66" ca="1" si="0">RANDBETWEEN(10000, 999999999)</f>
-        <v>30751941</v>
+        <v>712639313</v>
       </c>
       <c r="J3" s="1">
         <v>10</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>809945577</v>
+        <v>16572122</v>
       </c>
       <c r="J4" s="1">
         <v>10</v>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>273716082</v>
+        <v>499167949</v>
       </c>
       <c r="J5" s="1">
         <v>10</v>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>450029226</v>
+        <v>382438081</v>
       </c>
       <c r="J6" s="1">
         <v>10</v>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>600493946</v>
+        <v>16866156</v>
       </c>
       <c r="J7" s="1">
         <v>10</v>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41083556</v>
+        <v>166811606</v>
       </c>
       <c r="J8" s="1">
         <v>10</v>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>743168612</v>
+        <v>171681057</v>
       </c>
       <c r="J9" s="1">
         <v>10</v>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>507126013</v>
+        <v>861908589</v>
       </c>
       <c r="J10" s="1">
         <v>10</v>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>679435351</v>
+        <v>679160087</v>
       </c>
       <c r="J11" s="1">
         <v>10</v>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>672480157</v>
+        <v>799138825</v>
       </c>
       <c r="J12" s="1">
         <v>10</v>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>870685116</v>
+        <v>827650866</v>
       </c>
       <c r="J13" s="1">
         <v>10</v>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>940813936</v>
+        <v>944129105</v>
       </c>
       <c r="J14" s="1">
         <v>10</v>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>898450770</v>
+        <v>562422811</v>
       </c>
       <c r="J15" s="1">
         <v>10</v>
@@ -2114,7 +2114,7 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>160167894</v>
+        <v>837549753</v>
       </c>
       <c r="J16" s="1">
         <v>10</v>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>294267594</v>
+        <v>555711927</v>
       </c>
       <c r="J17" s="1">
         <v>10</v>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>645512862</v>
+        <v>97961257</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>206513955</v>
+        <v>898702149</v>
       </c>
       <c r="J19" s="1">
         <v>10</v>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>480817336</v>
+        <v>716822292</v>
       </c>
       <c r="J20" s="1">
         <v>10</v>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="I21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>221135986</v>
+        <v>313457969</v>
       </c>
       <c r="J21" s="1">
         <v>10</v>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>179214977</v>
+        <v>234468338</v>
       </c>
       <c r="J22" s="1">
         <v>10</v>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>215855498</v>
+        <v>358522147</v>
       </c>
       <c r="J23" s="1">
         <v>10</v>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>507704743</v>
+        <v>467149079</v>
       </c>
       <c r="J24" s="1">
         <v>10</v>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>253745568</v>
+        <v>34911367</v>
       </c>
       <c r="J25" s="1">
         <v>10</v>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>79978683</v>
+        <v>28507764</v>
       </c>
       <c r="J26" s="1">
         <v>10</v>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="I27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>206342354</v>
+        <v>872755870</v>
       </c>
       <c r="J27" s="1">
         <v>10</v>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="I28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>987772960</v>
+        <v>11525812</v>
       </c>
       <c r="J28" s="1">
         <v>10</v>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="I29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3799461</v>
+        <v>729493490</v>
       </c>
       <c r="J29" s="1">
         <v>10</v>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="I30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>900936619</v>
+        <v>815220135</v>
       </c>
       <c r="J30" s="1">
         <v>10</v>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>490236409</v>
+        <v>461204293</v>
       </c>
       <c r="J31" s="1">
         <v>10</v>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>812705650</v>
+        <v>998334968</v>
       </c>
       <c r="J32" s="1">
         <v>10</v>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="I33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2043392</v>
+        <v>638462267</v>
       </c>
       <c r="J33" s="1">
         <v>10</v>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>345458951</v>
+        <v>331589032</v>
       </c>
       <c r="J34" s="1">
         <v>10</v>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="I35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>254337194</v>
+        <v>272327835</v>
       </c>
       <c r="J35" s="1">
         <v>10</v>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="I36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>850878419</v>
+        <v>621450918</v>
       </c>
       <c r="J36" s="1">
         <v>10</v>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="I37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>102194926</v>
+        <v>609084014</v>
       </c>
       <c r="J37" s="1">
         <v>10</v>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="I38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>582356511</v>
+        <v>522473943</v>
       </c>
       <c r="J38" s="1">
         <v>10</v>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="I39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>976587440</v>
+        <v>201354654</v>
       </c>
       <c r="J39" s="1">
         <v>10</v>
@@ -3143,7 +3143,7 @@
       </c>
       <c r="I40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>340777076</v>
+        <v>457344222</v>
       </c>
       <c r="J40" s="1">
         <v>10</v>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="I41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>694469522</v>
+        <v>497135078</v>
       </c>
       <c r="J41" s="1">
         <v>10</v>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="I42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>714940225</v>
+        <v>857017730</v>
       </c>
       <c r="J42" s="1">
         <v>10</v>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="I43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>322041168</v>
+        <v>762526902</v>
       </c>
       <c r="J43" s="1">
         <v>10</v>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="I44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>787489256</v>
+        <v>844444056</v>
       </c>
       <c r="J44" s="1">
         <v>10</v>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="I45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>886399247</v>
+        <v>399453277</v>
       </c>
       <c r="J45" s="1">
         <v>10</v>
@@ -3398,7 +3398,7 @@
       </c>
       <c r="I46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>968158827</v>
+        <v>895611349</v>
       </c>
       <c r="J46" s="1">
         <v>10</v>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="I47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>480097086</v>
+        <v>45834290</v>
       </c>
       <c r="J47" s="1">
         <v>10</v>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="I48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>968725436</v>
+        <v>478286887</v>
       </c>
       <c r="J48" s="1">
         <v>10</v>
@@ -3527,7 +3527,7 @@
       </c>
       <c r="I49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>168342868</v>
+        <v>732602838</v>
       </c>
       <c r="J49" s="1">
         <v>10</v>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="I50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>971024497</v>
+        <v>156814695</v>
       </c>
       <c r="J50" s="1">
         <v>10</v>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="I51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>895561231</v>
+        <v>709759611</v>
       </c>
       <c r="J51" s="1">
         <v>10</v>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="I52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>670190017</v>
+        <v>882443907</v>
       </c>
       <c r="J52" s="1">
         <v>10</v>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="I53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>214530231</v>
+        <v>521477089</v>
       </c>
       <c r="J53" s="1">
         <v>10</v>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="I54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>525009786</v>
+        <v>346077147</v>
       </c>
       <c r="J54" s="1">
         <v>10</v>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="I55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>182599138</v>
+        <v>805360981</v>
       </c>
       <c r="J55" s="1">
         <v>10</v>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="I56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>905874300</v>
+        <v>555074378</v>
       </c>
       <c r="J56" s="1">
         <v>10</v>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="I57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>456580857</v>
+        <v>446789667</v>
       </c>
       <c r="J57" s="1">
         <v>10</v>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="I58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>629495136</v>
+        <v>72641372</v>
       </c>
       <c r="J58" s="1">
         <v>10</v>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="I59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>23073038</v>
+        <v>443980505</v>
       </c>
       <c r="J59" s="1">
         <v>10</v>
@@ -3998,7 +3998,7 @@
       </c>
       <c r="I60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>889441872</v>
+        <v>213077318</v>
       </c>
       <c r="J60" s="1">
         <v>10</v>
@@ -4040,7 +4040,7 @@
       </c>
       <c r="I61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>789984656</v>
+        <v>202696099</v>
       </c>
       <c r="J61" s="1">
         <v>10</v>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="I62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>212242629</v>
+        <v>514673278</v>
       </c>
       <c r="J62" s="1">
         <v>10</v>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="I63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>144557243</v>
+        <v>139708597</v>
       </c>
       <c r="J63" s="1">
         <v>10</v>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="I64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>768581852</v>
+        <v>487080006</v>
       </c>
       <c r="J64" s="1">
         <v>10</v>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="I65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>543033277</v>
+        <v>574737036</v>
       </c>
       <c r="J65" s="1">
         <v>10</v>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="I66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>736840908</v>
+        <v>812772915</v>
       </c>
       <c r="J66" s="1">
         <v>10</v>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="I67" s="1">
         <f t="shared" ref="I67:I130" ca="1" si="1">RANDBETWEEN(10000, 999999999)</f>
-        <v>207546165</v>
+        <v>222669337</v>
       </c>
       <c r="J67" s="1">
         <v>10</v>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="I68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>895318681</v>
+        <v>713547083</v>
       </c>
       <c r="J68" s="1">
         <v>10</v>
@@ -4382,7 +4382,7 @@
       </c>
       <c r="I69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>327620465</v>
+        <v>406782853</v>
       </c>
       <c r="J69" s="1">
         <v>10</v>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="I70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>795803220</v>
+        <v>77283303</v>
       </c>
       <c r="J70" s="1">
         <v>10</v>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="I71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>17434278</v>
+        <v>847134617</v>
       </c>
       <c r="J71" s="1">
         <v>10</v>
@@ -4508,7 +4508,7 @@
       </c>
       <c r="I72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>547891383</v>
+        <v>964910038</v>
       </c>
       <c r="J72" s="1">
         <v>10</v>
@@ -4553,7 +4553,7 @@
       </c>
       <c r="I73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>705363431</v>
+        <v>638692113</v>
       </c>
       <c r="J73" s="1">
         <v>10</v>
@@ -4595,7 +4595,7 @@
       </c>
       <c r="I74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>15758164</v>
+        <v>466216070</v>
       </c>
       <c r="J74" s="1">
         <v>10</v>
@@ -4637,7 +4637,7 @@
       </c>
       <c r="I75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>285868334</v>
+        <v>641331748</v>
       </c>
       <c r="J75" s="1">
         <v>10</v>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="I76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>289860951</v>
+        <v>393268863</v>
       </c>
       <c r="J76" s="1">
         <v>10</v>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="I77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>412441752</v>
+        <v>145252197</v>
       </c>
       <c r="J77" s="1">
         <v>10</v>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="I78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>568415421</v>
+        <v>684025122</v>
       </c>
       <c r="J78" s="1">
         <v>10</v>
@@ -4811,7 +4811,7 @@
       </c>
       <c r="I79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>888526642</v>
+        <v>403016607</v>
       </c>
       <c r="J79" s="1">
         <v>10</v>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="I80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>442194917</v>
+        <v>288135862</v>
       </c>
       <c r="J80" s="1">
         <v>10</v>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="I81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>758928846</v>
+        <v>89858026</v>
       </c>
       <c r="J81" s="1">
         <v>10</v>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="I82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>422412059</v>
+        <v>180032652</v>
       </c>
       <c r="J82" s="1">
         <v>10</v>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="I83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>834979789</v>
+        <v>118814403</v>
       </c>
       <c r="J83" s="1">
         <v>10</v>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="I84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>981375192</v>
+        <v>553185327</v>
       </c>
       <c r="J84" s="1">
         <v>10</v>
@@ -5066,7 +5066,7 @@
       </c>
       <c r="I85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>722668259</v>
+        <v>939461555</v>
       </c>
       <c r="J85" s="1">
         <v>10</v>
@@ -5108,7 +5108,7 @@
       </c>
       <c r="I86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>289386993</v>
+        <v>701131355</v>
       </c>
       <c r="J86" s="1">
         <v>10</v>
@@ -5150,7 +5150,7 @@
       </c>
       <c r="I87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>267454391</v>
+        <v>892876419</v>
       </c>
       <c r="J87" s="1">
         <v>10</v>
@@ -5192,7 +5192,7 @@
       </c>
       <c r="I88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>19422213</v>
+        <v>522934058</v>
       </c>
       <c r="J88" s="1">
         <v>10</v>
@@ -5237,7 +5237,7 @@
       </c>
       <c r="I89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>399744229</v>
+        <v>94113747</v>
       </c>
       <c r="J89" s="1">
         <v>10</v>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="I90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>46092920</v>
+        <v>45984708</v>
       </c>
       <c r="J90" s="1">
         <v>10</v>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="I91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>902450963</v>
+        <v>240483775</v>
       </c>
       <c r="J91" s="1">
         <v>10</v>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="I92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>102738191</v>
+        <v>657246837</v>
       </c>
       <c r="J92" s="1">
         <v>10</v>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="I93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>641009909</v>
+        <v>452650124</v>
       </c>
       <c r="J93" s="1">
         <v>10</v>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="I94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>883191100</v>
+        <v>507560916</v>
       </c>
       <c r="J94" s="1">
         <v>10</v>
@@ -5492,7 +5492,7 @@
       </c>
       <c r="I95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>898431312</v>
+        <v>493483729</v>
       </c>
       <c r="J95" s="1">
         <v>10</v>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="I96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>427926908</v>
+        <v>734197782</v>
       </c>
       <c r="J96" s="1">
         <v>10</v>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="I97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>895841683</v>
+        <v>200686733</v>
       </c>
       <c r="J97" s="1">
         <v>10</v>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="I98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>159441286</v>
+        <v>15711510</v>
       </c>
       <c r="J98" s="1">
         <v>10</v>
@@ -5666,7 +5666,7 @@
       </c>
       <c r="I99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>255393321</v>
+        <v>33676816</v>
       </c>
       <c r="J99" s="1">
         <v>10</v>
@@ -5708,7 +5708,7 @@
       </c>
       <c r="I100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>906660297</v>
+        <v>69005753</v>
       </c>
       <c r="J100" s="1">
         <v>10</v>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="I101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>313841732</v>
+        <v>337506105</v>
       </c>
       <c r="J101" s="1">
         <v>10</v>
@@ -5792,7 +5792,7 @@
       </c>
       <c r="I102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>547601894</v>
+        <v>132311435</v>
       </c>
       <c r="J102" s="1">
         <v>10</v>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="I103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>514375790</v>
+        <v>105461003</v>
       </c>
       <c r="J103" s="1">
         <v>10</v>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="I104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>229673797</v>
+        <v>366852788</v>
       </c>
       <c r="J104" s="1">
         <v>10</v>
@@ -5921,7 +5921,7 @@
       </c>
       <c r="I105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>202909326</v>
+        <v>979668662</v>
       </c>
       <c r="J105" s="1">
         <v>10</v>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="I106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>498505261</v>
+        <v>368181240</v>
       </c>
       <c r="J106" s="1">
         <v>10</v>
@@ -6005,7 +6005,7 @@
       </c>
       <c r="I107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>372957562</v>
+        <v>569877319</v>
       </c>
       <c r="J107" s="1">
         <v>10</v>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="I108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>768855842</v>
+        <v>950109160</v>
       </c>
       <c r="J108" s="1">
         <v>10</v>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="I109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>61152844</v>
+        <v>490270569</v>
       </c>
       <c r="J109" s="1">
         <v>10</v>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="I110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>713581603</v>
+        <v>609723466</v>
       </c>
       <c r="J110" s="1">
         <v>10</v>
@@ -6176,7 +6176,7 @@
       </c>
       <c r="I111" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>989831777</v>
+        <v>992907997</v>
       </c>
       <c r="J111" s="1">
         <v>10</v>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="I112" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>145158918</v>
+        <v>740575</v>
       </c>
       <c r="J112" s="1">
         <v>10</v>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="I113" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>885487508</v>
+        <v>747128782</v>
       </c>
       <c r="J113" s="1">
         <v>10</v>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="I114" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>566704245</v>
+        <v>642983311</v>
       </c>
       <c r="J114" s="1">
         <v>10</v>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="I115" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>24838487</v>
+        <v>125837685</v>
       </c>
       <c r="J115" s="1">
         <v>10</v>
@@ -6389,7 +6389,7 @@
       </c>
       <c r="I116" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>286002585</v>
+        <v>633239549</v>
       </c>
       <c r="J116" s="1">
         <v>10</v>
@@ -6431,7 +6431,7 @@
       </c>
       <c r="I117" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>274725884</v>
+        <v>361636177</v>
       </c>
       <c r="J117" s="1">
         <v>10</v>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="I118" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>288447827</v>
+        <v>814755204</v>
       </c>
       <c r="J118" s="1">
         <v>10</v>
@@ -6521,7 +6521,7 @@
       </c>
       <c r="I119" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>412474613</v>
+        <v>883357217</v>
       </c>
       <c r="J119" s="1">
         <v>10</v>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="I120" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>923884427</v>
+        <v>82780912</v>
       </c>
       <c r="J120" s="1">
         <v>10</v>
@@ -6605,7 +6605,7 @@
       </c>
       <c r="I121" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>559692358</v>
+        <v>605233158</v>
       </c>
       <c r="J121" s="1">
         <v>10</v>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="I122" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>822440947</v>
+        <v>505706160</v>
       </c>
       <c r="J122" s="1" t="s">
         <v>9</v>
@@ -6695,7 +6695,7 @@
       </c>
       <c r="I123" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>236869139</v>
+        <v>736065542</v>
       </c>
       <c r="J123" s="1">
         <v>10</v>
@@ -6740,7 +6740,7 @@
       </c>
       <c r="I124" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>33726421</v>
+        <v>383624783</v>
       </c>
       <c r="J124" s="1">
         <v>10</v>
@@ -6782,7 +6782,7 @@
       </c>
       <c r="I125" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>898893407</v>
+        <v>862350601</v>
       </c>
       <c r="J125" s="1">
         <v>10</v>
@@ -6824,7 +6824,7 @@
       </c>
       <c r="I126" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44422427</v>
+        <v>105021027</v>
       </c>
       <c r="J126" s="1">
         <v>10</v>
@@ -6866,7 +6866,7 @@
       </c>
       <c r="I127" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>236145228</v>
+        <v>81494586</v>
       </c>
       <c r="J127" s="1">
         <v>10</v>
@@ -6908,7 +6908,7 @@
       </c>
       <c r="I128" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>633212729</v>
+        <v>841406877</v>
       </c>
       <c r="J128" s="1">
         <v>10</v>
@@ -6950,7 +6950,7 @@
       </c>
       <c r="I129" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>76651192</v>
+        <v>460331503</v>
       </c>
       <c r="J129" s="1">
         <v>10</v>
@@ -6995,7 +6995,7 @@
       </c>
       <c r="I130" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>385810698</v>
+        <v>815718416</v>
       </c>
       <c r="J130" s="1">
         <v>10</v>
@@ -7037,7 +7037,7 @@
       </c>
       <c r="I131" s="1">
         <f t="shared" ref="I131:I194" ca="1" si="2">RANDBETWEEN(10000, 999999999)</f>
-        <v>47932353</v>
+        <v>120936844</v>
       </c>
       <c r="J131" s="1">
         <v>10</v>
@@ -7079,7 +7079,7 @@
       </c>
       <c r="I132" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>293056477</v>
+        <v>750642237</v>
       </c>
       <c r="J132" s="1">
         <v>10</v>
@@ -7121,7 +7121,7 @@
       </c>
       <c r="I133" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>363143147</v>
+        <v>142721654</v>
       </c>
       <c r="J133" s="1">
         <v>10</v>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="I134" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>141353942</v>
+        <v>672781834</v>
       </c>
       <c r="J134" s="1">
         <v>10</v>
@@ -7208,7 +7208,7 @@
       </c>
       <c r="I135" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>144857299</v>
+        <v>749666677</v>
       </c>
       <c r="J135" s="1">
         <v>10</v>
@@ -7250,7 +7250,7 @@
       </c>
       <c r="I136" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>921178563</v>
+        <v>757884608</v>
       </c>
       <c r="J136" s="1">
         <v>10</v>
@@ -7292,7 +7292,7 @@
       </c>
       <c r="I137" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>114758562</v>
+        <v>939091921</v>
       </c>
       <c r="J137" s="1">
         <v>10</v>
@@ -7334,7 +7334,7 @@
       </c>
       <c r="I138" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>943048865</v>
+        <v>328882294</v>
       </c>
       <c r="J138" s="1">
         <v>10</v>
@@ -7382,7 +7382,7 @@
       </c>
       <c r="I139" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>872284708</v>
+        <v>44949736</v>
       </c>
       <c r="J139" s="1">
         <v>10</v>
@@ -7424,7 +7424,7 @@
       </c>
       <c r="I140" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>266419514</v>
+        <v>362090387</v>
       </c>
       <c r="J140" s="1">
         <v>10</v>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="I141" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>16448185</v>
+        <v>791067193</v>
       </c>
       <c r="J141" s="1">
         <v>10</v>
@@ -7508,7 +7508,7 @@
       </c>
       <c r="I142" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>827469724</v>
+        <v>407188729</v>
       </c>
       <c r="J142" s="1">
         <v>10</v>
@@ -7550,7 +7550,7 @@
       </c>
       <c r="I143" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>993604029</v>
+        <v>802622797</v>
       </c>
       <c r="J143" s="1">
         <v>10</v>
@@ -7595,7 +7595,7 @@
       </c>
       <c r="I144" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>419897957</v>
+        <v>311157288</v>
       </c>
       <c r="J144" s="1">
         <v>10</v>
@@ -7637,7 +7637,7 @@
       </c>
       <c r="I145" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>25275797</v>
+        <v>148440576</v>
       </c>
       <c r="J145" s="1">
         <v>10</v>
@@ -7679,7 +7679,7 @@
       </c>
       <c r="I146" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>417205696</v>
+        <v>997265996</v>
       </c>
       <c r="J146" s="1">
         <v>10</v>
@@ -7721,7 +7721,7 @@
       </c>
       <c r="I147" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>745521558</v>
+        <v>783619519</v>
       </c>
       <c r="J147" s="1">
         <v>10</v>
@@ -7763,7 +7763,7 @@
       </c>
       <c r="I148" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>390611576</v>
+        <v>647544992</v>
       </c>
       <c r="J148" s="1">
         <v>10</v>
@@ -7805,7 +7805,7 @@
       </c>
       <c r="I149" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>110179296</v>
+        <v>676257196</v>
       </c>
       <c r="J149" s="1">
         <v>10</v>
@@ -7850,7 +7850,7 @@
       </c>
       <c r="I150" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>80796791</v>
+        <v>663373617</v>
       </c>
       <c r="J150" s="1">
         <v>10</v>
@@ -7892,7 +7892,7 @@
       </c>
       <c r="I151" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>118458358</v>
+        <v>921835429</v>
       </c>
       <c r="J151" s="1">
         <v>10</v>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="I152" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>322959240</v>
+        <v>915333310</v>
       </c>
       <c r="J152" s="1">
         <v>10</v>
@@ -7976,7 +7976,7 @@
       </c>
       <c r="I153" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>815367574</v>
+        <v>513283400</v>
       </c>
       <c r="J153" s="1">
         <v>10</v>
@@ -8021,7 +8021,7 @@
       </c>
       <c r="I154" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>638840997</v>
+        <v>914771421</v>
       </c>
       <c r="J154" s="1">
         <v>10</v>
@@ -8063,7 +8063,7 @@
       </c>
       <c r="I155" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>401662825</v>
+        <v>908945747</v>
       </c>
       <c r="J155" s="1">
         <v>10</v>
@@ -8105,7 +8105,7 @@
       </c>
       <c r="I156" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>261303508</v>
+        <v>694168536</v>
       </c>
       <c r="J156" s="1">
         <v>10</v>
@@ -8147,7 +8147,7 @@
       </c>
       <c r="I157" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>839903401</v>
+        <v>136440553</v>
       </c>
       <c r="J157" s="1">
         <v>10</v>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="I158" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>494950985</v>
+        <v>619720802</v>
       </c>
       <c r="J158" s="1">
         <v>10</v>
@@ -8237,7 +8237,7 @@
       </c>
       <c r="I159" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>675400652</v>
+        <v>980567024</v>
       </c>
       <c r="J159" s="1">
         <v>10</v>
@@ -8279,7 +8279,7 @@
       </c>
       <c r="I160" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>996174350</v>
+        <v>155444710</v>
       </c>
       <c r="J160" s="1">
         <v>10</v>
@@ -8321,7 +8321,7 @@
       </c>
       <c r="I161" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>805548045</v>
+        <v>105757679</v>
       </c>
       <c r="J161" s="1">
         <v>10</v>
@@ -8363,7 +8363,7 @@
       </c>
       <c r="I162" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>393341297</v>
+        <v>453976269</v>
       </c>
       <c r="J162" s="1">
         <v>10</v>
@@ -8405,7 +8405,7 @@
       </c>
       <c r="I163" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>679815980</v>
+        <v>282591947</v>
       </c>
       <c r="J163" s="1">
         <v>10</v>
@@ -8450,7 +8450,7 @@
       </c>
       <c r="I164" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>180427492</v>
+        <v>377098486</v>
       </c>
       <c r="J164" s="1">
         <v>10</v>
@@ -8492,7 +8492,7 @@
       </c>
       <c r="I165" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>727173325</v>
+        <v>41222685</v>
       </c>
       <c r="J165" s="1">
         <v>10</v>
@@ -8534,7 +8534,7 @@
       </c>
       <c r="I166" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>292170908</v>
+        <v>932115984</v>
       </c>
       <c r="J166" s="1">
         <v>10</v>
@@ -8576,7 +8576,7 @@
       </c>
       <c r="I167" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>846203375</v>
+        <v>228133459</v>
       </c>
       <c r="J167" s="1">
         <v>10</v>
@@ -8618,7 +8618,7 @@
       </c>
       <c r="I168" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>758444416</v>
+        <v>631137297</v>
       </c>
       <c r="J168" s="1">
         <v>10</v>
@@ -8660,7 +8660,7 @@
       </c>
       <c r="I169" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>51681408</v>
+        <v>88524107</v>
       </c>
       <c r="J169" s="1">
         <v>10</v>
@@ -8705,7 +8705,7 @@
       </c>
       <c r="I170" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>976259301</v>
+        <v>110553316</v>
       </c>
       <c r="J170" s="1">
         <v>10</v>
@@ -8747,7 +8747,7 @@
       </c>
       <c r="I171" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>639487357</v>
+        <v>122246876</v>
       </c>
       <c r="J171" s="1">
         <v>10</v>
@@ -8789,7 +8789,7 @@
       </c>
       <c r="I172" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>376063135</v>
+        <v>661862583</v>
       </c>
       <c r="J172" s="1">
         <v>10</v>
@@ -8831,7 +8831,7 @@
       </c>
       <c r="I173" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>643537201</v>
+        <v>116099191</v>
       </c>
       <c r="J173" s="1">
         <v>10</v>
@@ -8876,7 +8876,7 @@
       </c>
       <c r="I174" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>118705106</v>
+        <v>223152634</v>
       </c>
       <c r="J174" s="1">
         <v>10</v>
@@ -8918,7 +8918,7 @@
       </c>
       <c r="I175" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>558943061</v>
+        <v>348717993</v>
       </c>
       <c r="J175" s="1">
         <v>10</v>
@@ -8960,7 +8960,7 @@
       </c>
       <c r="I176" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>120013876</v>
+        <v>334559890</v>
       </c>
       <c r="J176" s="1">
         <v>10</v>
@@ -9002,7 +9002,7 @@
       </c>
       <c r="I177" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>215894838</v>
+        <v>251364590</v>
       </c>
       <c r="J177" s="1">
         <v>10</v>
@@ -9044,7 +9044,7 @@
       </c>
       <c r="I178" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>58976211</v>
+        <v>601601931</v>
       </c>
       <c r="J178" s="1">
         <v>10</v>
@@ -9092,7 +9092,7 @@
       </c>
       <c r="I179" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>586276035</v>
+        <v>790045853</v>
       </c>
       <c r="J179" s="1">
         <v>10</v>
@@ -9134,7 +9134,7 @@
       </c>
       <c r="I180" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>492041997</v>
+        <v>402287434</v>
       </c>
       <c r="J180" s="1">
         <v>10</v>
@@ -9176,7 +9176,7 @@
       </c>
       <c r="I181" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>387660918</v>
+        <v>436986178</v>
       </c>
       <c r="J181" s="1">
         <v>10</v>
@@ -9218,7 +9218,7 @@
       </c>
       <c r="I182" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>892476495</v>
+        <v>143141681</v>
       </c>
       <c r="J182" s="1">
         <v>10</v>
@@ -9260,7 +9260,7 @@
       </c>
       <c r="I183" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>81588147</v>
+        <v>806340374</v>
       </c>
       <c r="J183" s="1">
         <v>10</v>
@@ -9305,7 +9305,7 @@
       </c>
       <c r="I184" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>195090741</v>
+        <v>25144739</v>
       </c>
       <c r="J184" s="1">
         <v>10</v>
@@ -9347,7 +9347,7 @@
       </c>
       <c r="I185" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>841423113</v>
+        <v>414654109</v>
       </c>
       <c r="J185" s="1">
         <v>10</v>
@@ -9389,7 +9389,7 @@
       </c>
       <c r="I186" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>207086794</v>
+        <v>921693651</v>
       </c>
       <c r="J186" s="1">
         <v>10</v>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="I187" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>267350424</v>
+        <v>272161768</v>
       </c>
       <c r="J187" s="1">
         <v>10</v>
@@ -9473,7 +9473,7 @@
       </c>
       <c r="I188" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>765035003</v>
+        <v>680306898</v>
       </c>
       <c r="J188" s="1">
         <v>10</v>
@@ -9515,7 +9515,7 @@
       </c>
       <c r="I189" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>135450279</v>
+        <v>781348434</v>
       </c>
       <c r="J189" s="1">
         <v>10</v>
@@ -9560,7 +9560,7 @@
       </c>
       <c r="I190" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>30764789</v>
+        <v>162741133</v>
       </c>
       <c r="J190" s="1">
         <v>10</v>
@@ -9602,7 +9602,7 @@
       </c>
       <c r="I191" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>816217469</v>
+        <v>208324202</v>
       </c>
       <c r="J191" s="1">
         <v>10</v>
@@ -9644,7 +9644,7 @@
       </c>
       <c r="I192" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>612132712</v>
+        <v>840548857</v>
       </c>
       <c r="J192" s="1">
         <v>10</v>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="I193" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>313014678</v>
+        <v>618960203</v>
       </c>
       <c r="J193" s="1">
         <v>10</v>
@@ -9731,7 +9731,7 @@
       </c>
       <c r="I194" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>535358395</v>
+        <v>913124220</v>
       </c>
       <c r="J194" s="1">
         <v>10</v>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="I195" s="1">
         <f t="shared" ref="I195:I258" ca="1" si="3">RANDBETWEEN(10000, 999999999)</f>
-        <v>397917150</v>
+        <v>781787376</v>
       </c>
       <c r="J195" s="1">
         <v>10</v>
@@ -9815,7 +9815,7 @@
       </c>
       <c r="I196" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>648908145</v>
+        <v>340179644</v>
       </c>
       <c r="J196" s="1">
         <v>10</v>
@@ -9857,7 +9857,7 @@
       </c>
       <c r="I197" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>65346387</v>
+        <v>562591118</v>
       </c>
       <c r="J197" s="1">
         <v>10</v>
@@ -9899,7 +9899,7 @@
       </c>
       <c r="I198" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>277461883</v>
+        <v>636834140</v>
       </c>
       <c r="J198" s="1">
         <v>10</v>
@@ -9947,7 +9947,7 @@
       </c>
       <c r="I199" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>128877670</v>
+        <v>960712313</v>
       </c>
       <c r="J199" s="1">
         <v>10</v>
@@ -9989,7 +9989,7 @@
       </c>
       <c r="I200" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>963008941</v>
+        <v>509400072</v>
       </c>
       <c r="J200" s="1">
         <v>10</v>
@@ -10031,7 +10031,7 @@
       </c>
       <c r="I201" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>921269555</v>
+        <v>520917588</v>
       </c>
       <c r="J201" s="1">
         <v>10</v>
@@ -10073,7 +10073,7 @@
       </c>
       <c r="I202" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>729696945</v>
+        <v>627091076</v>
       </c>
       <c r="J202" s="1">
         <v>10</v>
@@ -10115,7 +10115,7 @@
       </c>
       <c r="I203" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>951576542</v>
+        <v>567235351</v>
       </c>
       <c r="J203" s="1">
         <v>10</v>
@@ -10160,7 +10160,7 @@
       </c>
       <c r="I204" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>489469983</v>
+        <v>792265721</v>
       </c>
       <c r="J204" s="1">
         <v>10</v>
@@ -10202,7 +10202,7 @@
       </c>
       <c r="I205" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>269308195</v>
+        <v>625320235</v>
       </c>
       <c r="J205" s="1">
         <v>10</v>
@@ -10244,7 +10244,7 @@
       </c>
       <c r="I206" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>269596710</v>
+        <v>238252839</v>
       </c>
       <c r="J206" s="1">
         <v>10</v>
@@ -10286,7 +10286,7 @@
       </c>
       <c r="I207" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>893543235</v>
+        <v>887083965</v>
       </c>
       <c r="J207" s="1">
         <v>10</v>
@@ -10328,7 +10328,7 @@
       </c>
       <c r="I208" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>873162938</v>
+        <v>180509369</v>
       </c>
       <c r="J208" s="1">
         <v>10</v>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="I209" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>852320958</v>
+        <v>707981957</v>
       </c>
       <c r="J209" s="1">
         <v>10</v>
@@ -10415,7 +10415,7 @@
       </c>
       <c r="I210" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>585205612</v>
+        <v>517506718</v>
       </c>
       <c r="J210" s="1">
         <v>10</v>
@@ -10457,7 +10457,7 @@
       </c>
       <c r="I211" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>593162227</v>
+        <v>34653413</v>
       </c>
       <c r="J211" s="1">
         <v>10</v>
@@ -10499,7 +10499,7 @@
       </c>
       <c r="I212" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>154335304</v>
+        <v>663911861</v>
       </c>
       <c r="J212" s="1">
         <v>10</v>
@@ -10541,7 +10541,7 @@
       </c>
       <c r="I213" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>314801014</v>
+        <v>359011380</v>
       </c>
       <c r="J213" s="1">
         <v>10</v>
@@ -10586,7 +10586,7 @@
       </c>
       <c r="I214" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>415987437</v>
+        <v>161118030</v>
       </c>
       <c r="J214" s="1">
         <v>10</v>
@@ -10628,7 +10628,7 @@
       </c>
       <c r="I215" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>562235478</v>
+        <v>426106916</v>
       </c>
       <c r="J215" s="1">
         <v>10</v>
@@ -10670,7 +10670,7 @@
       </c>
       <c r="I216" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>194301586</v>
+        <v>673455538</v>
       </c>
       <c r="J216" s="1">
         <v>10</v>
@@ -10712,7 +10712,7 @@
       </c>
       <c r="I217" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>57543367</v>
+        <v>910780741</v>
       </c>
       <c r="J217" s="1">
         <v>10</v>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="I218" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>246713722</v>
+        <v>868402780</v>
       </c>
       <c r="J218" s="1">
         <v>10</v>
@@ -10802,7 +10802,7 @@
       </c>
       <c r="I219" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>694949276</v>
+        <v>548700503</v>
       </c>
       <c r="J219" s="1">
         <v>10</v>
@@ -10844,7 +10844,7 @@
       </c>
       <c r="I220" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>298064284</v>
+        <v>82759777</v>
       </c>
       <c r="J220" s="1">
         <v>10</v>
@@ -10886,7 +10886,7 @@
       </c>
       <c r="I221" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>680075660</v>
+        <v>678016888</v>
       </c>
       <c r="J221" s="1">
         <v>10</v>
@@ -10928,7 +10928,7 @@
       </c>
       <c r="I222" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>614548009</v>
+        <v>733518561</v>
       </c>
       <c r="J222" s="1">
         <v>10</v>
@@ -10970,7 +10970,7 @@
       </c>
       <c r="I223" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>539306049</v>
+        <v>257837652</v>
       </c>
       <c r="J223" s="1">
         <v>10</v>
@@ -11015,7 +11015,7 @@
       </c>
       <c r="I224" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>129042654</v>
+        <v>914463031</v>
       </c>
       <c r="J224" s="1">
         <v>10</v>
@@ -11057,7 +11057,7 @@
       </c>
       <c r="I225" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>391435457</v>
+        <v>411668986</v>
       </c>
       <c r="J225" s="1">
         <v>10</v>
@@ -11099,7 +11099,7 @@
       </c>
       <c r="I226" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>806098885</v>
+        <v>193076304</v>
       </c>
       <c r="J226" s="1">
         <v>10</v>
@@ -11141,7 +11141,7 @@
       </c>
       <c r="I227" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>522939609</v>
+        <v>718779582</v>
       </c>
       <c r="J227" s="1">
         <v>10</v>
@@ -11183,7 +11183,7 @@
       </c>
       <c r="I228" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>344745825</v>
+        <v>203926146</v>
       </c>
       <c r="J228" s="1">
         <v>10</v>
@@ -11225,7 +11225,7 @@
       </c>
       <c r="I229" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>514828792</v>
+        <v>733339146</v>
       </c>
       <c r="J229" s="1">
         <v>10</v>
@@ -11270,7 +11270,7 @@
       </c>
       <c r="I230" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>929333286</v>
+        <v>51982535</v>
       </c>
       <c r="J230" s="1">
         <v>10</v>
@@ -11312,7 +11312,7 @@
       </c>
       <c r="I231" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>198195112</v>
+        <v>50585586</v>
       </c>
       <c r="J231" s="1">
         <v>10</v>
@@ -11354,7 +11354,7 @@
       </c>
       <c r="I232" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>952502234</v>
+        <v>216164571</v>
       </c>
       <c r="J232" s="1">
         <v>10</v>
@@ -11396,7 +11396,7 @@
       </c>
       <c r="I233" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>676141464</v>
+        <v>152820177</v>
       </c>
       <c r="J233" s="1">
         <v>10</v>
@@ -11441,7 +11441,7 @@
       </c>
       <c r="I234" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>450262616</v>
+        <v>327804652</v>
       </c>
       <c r="J234" s="1">
         <v>10</v>
@@ -11483,7 +11483,7 @@
       </c>
       <c r="I235" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>758408859</v>
+        <v>880550112</v>
       </c>
       <c r="J235" s="1">
         <v>10</v>
@@ -11525,7 +11525,7 @@
       </c>
       <c r="I236" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>183223399</v>
+        <v>416533483</v>
       </c>
       <c r="J236" s="1">
         <v>10</v>
@@ -11567,7 +11567,7 @@
       </c>
       <c r="I237" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>521483584</v>
+        <v>406273015</v>
       </c>
       <c r="J237" s="1">
         <v>10</v>
@@ -11609,7 +11609,7 @@
       </c>
       <c r="I238" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>708971753</v>
+        <v>647368304</v>
       </c>
       <c r="J238" s="1">
         <v>10</v>
@@ -11657,7 +11657,7 @@
       </c>
       <c r="I239" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>635012314</v>
+        <v>921136570</v>
       </c>
       <c r="J239" s="1">
         <v>10</v>
@@ -11699,7 +11699,7 @@
       </c>
       <c r="I240" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>375508774</v>
+        <v>466059559</v>
       </c>
       <c r="J240" s="1">
         <v>10</v>
@@ -11741,7 +11741,7 @@
       </c>
       <c r="I241" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>531002872</v>
+        <v>325214577</v>
       </c>
       <c r="J241" s="1">
         <v>10</v>
@@ -11783,7 +11783,7 @@
       </c>
       <c r="I242" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>690098173</v>
+        <v>799802118</v>
       </c>
       <c r="J242" s="1">
         <v>10</v>
@@ -11825,7 +11825,7 @@
       </c>
       <c r="I243" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>528393304</v>
+        <v>484813859</v>
       </c>
       <c r="J243" s="1" t="s">
         <v>9</v>
@@ -11873,7 +11873,7 @@
       </c>
       <c r="I244" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>834424761</v>
+        <v>405774722</v>
       </c>
       <c r="J244" s="1">
         <v>10</v>
@@ -11918,7 +11918,7 @@
       </c>
       <c r="I245" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>789670317</v>
+        <v>906036569</v>
       </c>
       <c r="J245" s="1">
         <v>10</v>
@@ -11960,7 +11960,7 @@
       </c>
       <c r="I246" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>774667783</v>
+        <v>731274972</v>
       </c>
       <c r="J246" s="1">
         <v>10</v>
@@ -12002,7 +12002,7 @@
       </c>
       <c r="I247" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>951231306</v>
+        <v>677869435</v>
       </c>
       <c r="J247" s="1">
         <v>10</v>
@@ -12044,7 +12044,7 @@
       </c>
       <c r="I248" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>779200389</v>
+        <v>675947841</v>
       </c>
       <c r="J248" s="1">
         <v>10</v>
@@ -12086,7 +12086,7 @@
       </c>
       <c r="I249" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>426459715</v>
+        <v>392462031</v>
       </c>
       <c r="J249" s="1">
         <v>10</v>
@@ -12128,7 +12128,7 @@
       </c>
       <c r="I250" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>583043984</v>
+        <v>256618930</v>
       </c>
       <c r="J250" s="1">
         <v>10</v>
@@ -12173,7 +12173,7 @@
       </c>
       <c r="I251" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>161995362</v>
+        <v>752976955</v>
       </c>
       <c r="J251" s="1">
         <v>10</v>
@@ -12215,7 +12215,7 @@
       </c>
       <c r="I252" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>855095107</v>
+        <v>289901443</v>
       </c>
       <c r="J252" s="1">
         <v>10</v>
@@ -12257,7 +12257,7 @@
       </c>
       <c r="I253" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>837608381</v>
+        <v>955759311</v>
       </c>
       <c r="J253" s="1">
         <v>10</v>
@@ -12299,7 +12299,7 @@
       </c>
       <c r="I254" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>503407974</v>
+        <v>523571071</v>
       </c>
       <c r="J254" s="1">
         <v>10</v>
@@ -12344,7 +12344,7 @@
       </c>
       <c r="I255" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>770900975</v>
+        <v>257235074</v>
       </c>
       <c r="J255" s="1">
         <v>10</v>
@@ -12386,7 +12386,7 @@
       </c>
       <c r="I256" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>863282704</v>
+        <v>111577062</v>
       </c>
       <c r="J256" s="1">
         <v>10</v>
@@ -12428,7 +12428,7 @@
       </c>
       <c r="I257" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>399761469</v>
+        <v>724301869</v>
       </c>
       <c r="J257" s="1">
         <v>10</v>
@@ -12470,7 +12470,7 @@
       </c>
       <c r="I258" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>542059458</v>
+        <v>98681242</v>
       </c>
       <c r="J258" s="1">
         <v>10</v>
@@ -12512,7 +12512,7 @@
       </c>
       <c r="I259" s="1">
         <f t="shared" ref="I259:I322" ca="1" si="4">RANDBETWEEN(10000, 999999999)</f>
-        <v>585123455</v>
+        <v>693201464</v>
       </c>
       <c r="J259" s="1">
         <v>10</v>
@@ -12560,7 +12560,7 @@
       </c>
       <c r="I260" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>430809491</v>
+        <v>189431570</v>
       </c>
       <c r="J260" s="1">
         <v>10</v>
@@ -12602,7 +12602,7 @@
       </c>
       <c r="I261" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>73206765</v>
+        <v>931225257</v>
       </c>
       <c r="J261" s="1">
         <v>10</v>
@@ -12644,7 +12644,7 @@
       </c>
       <c r="I262" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>117721817</v>
+        <v>693200515</v>
       </c>
       <c r="J262" s="1">
         <v>10</v>
@@ -12686,7 +12686,7 @@
       </c>
       <c r="I263" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>994017512</v>
+        <v>947405413</v>
       </c>
       <c r="J263" s="1">
         <v>10</v>
@@ -12728,7 +12728,7 @@
       </c>
       <c r="I264" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>29160037</v>
+        <v>431279751</v>
       </c>
       <c r="J264" s="1">
         <v>10</v>
@@ -12773,7 +12773,7 @@
       </c>
       <c r="I265" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>133245751</v>
+        <v>130131623</v>
       </c>
       <c r="J265" s="1">
         <v>10</v>
@@ -12815,7 +12815,7 @@
       </c>
       <c r="I266" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>996607580</v>
+        <v>547989221</v>
       </c>
       <c r="J266" s="1">
         <v>10</v>
@@ -12857,7 +12857,7 @@
       </c>
       <c r="I267" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>214591694</v>
+        <v>104394831</v>
       </c>
       <c r="J267" s="1">
         <v>10</v>
@@ -12899,7 +12899,7 @@
       </c>
       <c r="I268" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>780440707</v>
+        <v>386564089</v>
       </c>
       <c r="J268" s="1">
         <v>10</v>
@@ -12941,7 +12941,7 @@
       </c>
       <c r="I269" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>130460090</v>
+        <v>559237582</v>
       </c>
       <c r="J269" s="1">
         <v>10</v>
@@ -12983,7 +12983,7 @@
       </c>
       <c r="I270" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>586722756</v>
+        <v>888860437</v>
       </c>
       <c r="J270" s="1">
         <v>10</v>
@@ -13028,7 +13028,7 @@
       </c>
       <c r="I271" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>839503507</v>
+        <v>102186118</v>
       </c>
       <c r="J271" s="1">
         <v>10</v>
@@ -13070,7 +13070,7 @@
       </c>
       <c r="I272" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>394672460</v>
+        <v>536970915</v>
       </c>
       <c r="J272" s="1">
         <v>10</v>
@@ -13112,7 +13112,7 @@
       </c>
       <c r="I273" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1239305</v>
+        <v>458441055</v>
       </c>
       <c r="J273" s="1">
         <v>10</v>
@@ -13154,7 +13154,7 @@
       </c>
       <c r="I274" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>194946347</v>
+        <v>890301937</v>
       </c>
       <c r="J274" s="1">
         <v>10</v>
@@ -13199,7 +13199,7 @@
       </c>
       <c r="I275" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>338416324</v>
+        <v>833138445</v>
       </c>
       <c r="J275" s="1">
         <v>10</v>
@@ -13241,7 +13241,7 @@
       </c>
       <c r="I276" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>385386257</v>
+        <v>769771259</v>
       </c>
       <c r="J276" s="1">
         <v>10</v>
@@ -13283,7 +13283,7 @@
       </c>
       <c r="I277" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>49583594</v>
+        <v>183870421</v>
       </c>
       <c r="J277" s="1">
         <v>10</v>
@@ -13325,7 +13325,7 @@
       </c>
       <c r="I278" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>736544236</v>
+        <v>331784785</v>
       </c>
       <c r="J278" s="1">
         <v>10</v>
@@ -13367,7 +13367,7 @@
       </c>
       <c r="I279" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>881947842</v>
+        <v>546042410</v>
       </c>
       <c r="J279" s="1">
         <v>10</v>
@@ -13415,7 +13415,7 @@
       </c>
       <c r="I280" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>177279991</v>
+        <v>407353211</v>
       </c>
       <c r="J280" s="1">
         <v>10</v>
@@ -13457,7 +13457,7 @@
       </c>
       <c r="I281" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>89016104</v>
+        <v>370442173</v>
       </c>
       <c r="J281" s="1">
         <v>10</v>
@@ -13499,7 +13499,7 @@
       </c>
       <c r="I282" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>816680359</v>
+        <v>565239947</v>
       </c>
       <c r="J282" s="1">
         <v>10</v>
@@ -13541,7 +13541,7 @@
       </c>
       <c r="I283" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>757218451</v>
+        <v>222633151</v>
       </c>
       <c r="J283" s="1">
         <v>10</v>
@@ -13583,7 +13583,7 @@
       </c>
       <c r="I284" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>370205935</v>
+        <v>897810614</v>
       </c>
       <c r="J284" s="1">
         <v>10</v>
@@ -13628,7 +13628,7 @@
       </c>
       <c r="I285" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>501346915</v>
+        <v>321890199</v>
       </c>
       <c r="J285" s="1">
         <v>10</v>
@@ -13670,7 +13670,7 @@
       </c>
       <c r="I286" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>255171199</v>
+        <v>399862117</v>
       </c>
       <c r="J286" s="1">
         <v>10</v>
@@ -13712,7 +13712,7 @@
       </c>
       <c r="I287" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>122575515</v>
+        <v>554498970</v>
       </c>
       <c r="J287" s="1">
         <v>10</v>
@@ -13754,7 +13754,7 @@
       </c>
       <c r="I288" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>655988308</v>
+        <v>644040407</v>
       </c>
       <c r="J288" s="1">
         <v>10</v>
@@ -13796,7 +13796,7 @@
       </c>
       <c r="I289" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>181356805</v>
+        <v>15782539</v>
       </c>
       <c r="J289" s="1">
         <v>10</v>
@@ -13838,7 +13838,7 @@
       </c>
       <c r="I290" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>821932828</v>
+        <v>657780595</v>
       </c>
       <c r="J290" s="1">
         <v>10</v>
@@ -13883,7 +13883,7 @@
       </c>
       <c r="I291" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>808163543</v>
+        <v>941480984</v>
       </c>
       <c r="J291" s="1">
         <v>10</v>
@@ -13925,7 +13925,7 @@
       </c>
       <c r="I292" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>694768513</v>
+        <v>259708027</v>
       </c>
       <c r="J292" s="1">
         <v>10</v>
@@ -13967,7 +13967,7 @@
       </c>
       <c r="I293" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>832040136</v>
+        <v>68655485</v>
       </c>
       <c r="J293" s="1">
         <v>10</v>
@@ -14009,7 +14009,7 @@
       </c>
       <c r="I294" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>374171986</v>
+        <v>72707559</v>
       </c>
       <c r="J294" s="1">
         <v>10</v>
@@ -14054,7 +14054,7 @@
       </c>
       <c r="I295" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>385358428</v>
+        <v>610112429</v>
       </c>
       <c r="J295" s="1">
         <v>10</v>
@@ -14096,7 +14096,7 @@
       </c>
       <c r="I296" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>421717478</v>
+        <v>534266214</v>
       </c>
       <c r="J296" s="1">
         <v>10</v>
@@ -14138,7 +14138,7 @@
       </c>
       <c r="I297" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>416734422</v>
+        <v>696430513</v>
       </c>
       <c r="J297" s="1">
         <v>10</v>
@@ -14180,7 +14180,7 @@
       </c>
       <c r="I298" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>950330200</v>
+        <v>433117417</v>
       </c>
       <c r="J298" s="1">
         <v>10</v>
@@ -14222,7 +14222,7 @@
       </c>
       <c r="I299" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>742720305</v>
+        <v>649662578</v>
       </c>
       <c r="J299" s="1">
         <v>10</v>
@@ -14270,7 +14270,7 @@
       </c>
       <c r="I300" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>208662119</v>
+        <v>190282525</v>
       </c>
       <c r="J300" s="1">
         <v>10</v>
@@ -14312,7 +14312,7 @@
       </c>
       <c r="I301" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>345333687</v>
+        <v>466950813</v>
       </c>
       <c r="J301" s="1">
         <v>10</v>
@@ -14354,7 +14354,7 @@
       </c>
       <c r="I302" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>399104721</v>
+        <v>304953300</v>
       </c>
       <c r="J302" s="1">
         <v>10</v>
@@ -14396,7 +14396,7 @@
       </c>
       <c r="I303" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>21520151</v>
+        <v>207372828</v>
       </c>
       <c r="J303" s="1">
         <v>10</v>
@@ -14438,7 +14438,7 @@
       </c>
       <c r="I304" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>492181016</v>
+        <v>577293195</v>
       </c>
       <c r="J304" s="1">
         <v>10</v>
@@ -14483,7 +14483,7 @@
       </c>
       <c r="I305" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>934958758</v>
+        <v>582738502</v>
       </c>
       <c r="J305" s="1">
         <v>10</v>
@@ -14525,7 +14525,7 @@
       </c>
       <c r="I306" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>231369784</v>
+        <v>348954075</v>
       </c>
       <c r="J306" s="1">
         <v>10</v>
@@ -14567,7 +14567,7 @@
       </c>
       <c r="I307" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>220107658</v>
+        <v>162625612</v>
       </c>
       <c r="J307" s="1">
         <v>10</v>
@@ -14609,7 +14609,7 @@
       </c>
       <c r="I308" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>199590044</v>
+        <v>341708289</v>
       </c>
       <c r="J308" s="1">
         <v>10</v>
@@ -14651,7 +14651,7 @@
       </c>
       <c r="I309" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>21257256</v>
+        <v>540834905</v>
       </c>
       <c r="J309" s="1">
         <v>10</v>
@@ -14693,7 +14693,7 @@
       </c>
       <c r="I310" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>617892591</v>
+        <v>642046408</v>
       </c>
       <c r="J310" s="1">
         <v>10</v>
@@ -14738,7 +14738,7 @@
       </c>
       <c r="I311" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>789693706</v>
+        <v>546287164</v>
       </c>
       <c r="J311" s="1">
         <v>10</v>
@@ -14780,7 +14780,7 @@
       </c>
       <c r="I312" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>860490152</v>
+        <v>513960364</v>
       </c>
       <c r="J312" s="1">
         <v>10</v>
@@ -14822,7 +14822,7 @@
       </c>
       <c r="I313" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>666821786</v>
+        <v>978923035</v>
       </c>
       <c r="J313" s="1">
         <v>10</v>
@@ -14864,7 +14864,7 @@
       </c>
       <c r="I314" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>75068164</v>
+        <v>704652755</v>
       </c>
       <c r="J314" s="1">
         <v>10</v>
@@ -14909,7 +14909,7 @@
       </c>
       <c r="I315" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>367963732</v>
+        <v>575782622</v>
       </c>
       <c r="J315" s="1">
         <v>10</v>
@@ -14951,7 +14951,7 @@
       </c>
       <c r="I316" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>946174340</v>
+        <v>127659036</v>
       </c>
       <c r="J316" s="1">
         <v>10</v>
@@ -14993,7 +14993,7 @@
       </c>
       <c r="I317" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>814208410</v>
+        <v>198780540</v>
       </c>
       <c r="J317" s="1">
         <v>10</v>
@@ -15035,7 +15035,7 @@
       </c>
       <c r="I318" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>729640689</v>
+        <v>575985768</v>
       </c>
       <c r="J318" s="1">
         <v>10</v>
@@ -15077,7 +15077,7 @@
       </c>
       <c r="I319" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>486174688</v>
+        <v>840586320</v>
       </c>
       <c r="J319" s="1">
         <v>10</v>
@@ -15125,7 +15125,7 @@
       </c>
       <c r="I320" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>477431772</v>
+        <v>973686642</v>
       </c>
       <c r="J320" s="1">
         <v>10</v>
@@ -15167,7 +15167,7 @@
       </c>
       <c r="I321" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>470379281</v>
+        <v>963209024</v>
       </c>
       <c r="J321" s="1">
         <v>10</v>
@@ -15209,7 +15209,7 @@
       </c>
       <c r="I322" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>625215449</v>
+        <v>835732079</v>
       </c>
       <c r="J322" s="1">
         <v>10</v>
@@ -15251,7 +15251,7 @@
       </c>
       <c r="I323" s="1">
         <f t="shared" ref="I323:I363" ca="1" si="5">RANDBETWEEN(10000, 999999999)</f>
-        <v>682313177</v>
+        <v>922120690</v>
       </c>
       <c r="J323" s="1">
         <v>10</v>
@@ -15293,7 +15293,7 @@
       </c>
       <c r="I324" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>916714897</v>
+        <v>704029781</v>
       </c>
       <c r="J324" s="1">
         <v>10</v>
@@ -15338,7 +15338,7 @@
       </c>
       <c r="I325" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>25896278</v>
+        <v>861396197</v>
       </c>
       <c r="J325" s="1">
         <v>10</v>
@@ -15380,7 +15380,7 @@
       </c>
       <c r="I326" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>464543119</v>
+        <v>937249013</v>
       </c>
       <c r="J326" s="1">
         <v>10</v>
@@ -15422,7 +15422,7 @@
       </c>
       <c r="I327" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>929699035</v>
+        <v>442062931</v>
       </c>
       <c r="J327" s="1">
         <v>10</v>
@@ -15464,7 +15464,7 @@
       </c>
       <c r="I328" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>285124538</v>
+        <v>927171062</v>
       </c>
       <c r="J328" s="1">
         <v>10</v>
@@ -15506,7 +15506,7 @@
       </c>
       <c r="I329" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>364817590</v>
+        <v>708917117</v>
       </c>
       <c r="J329" s="1">
         <v>10</v>
@@ -15548,7 +15548,7 @@
       </c>
       <c r="I330" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>103026068</v>
+        <v>414801710</v>
       </c>
       <c r="J330" s="1">
         <v>10</v>
@@ -15593,7 +15593,7 @@
       </c>
       <c r="I331" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>95939729</v>
+        <v>649128891</v>
       </c>
       <c r="J331" s="1">
         <v>10</v>
@@ -15635,7 +15635,7 @@
       </c>
       <c r="I332" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>158036732</v>
+        <v>223144994</v>
       </c>
       <c r="J332" s="1">
         <v>10</v>
@@ -15677,7 +15677,7 @@
       </c>
       <c r="I333" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>248486350</v>
+        <v>777204373</v>
       </c>
       <c r="J333" s="1">
         <v>10</v>
@@ -15719,7 +15719,7 @@
       </c>
       <c r="I334" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>158373115</v>
+        <v>546093826</v>
       </c>
       <c r="J334" s="1">
         <v>10</v>
@@ -15764,7 +15764,7 @@
       </c>
       <c r="I335" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>319632477</v>
+        <v>128858133</v>
       </c>
       <c r="J335" s="1">
         <v>10</v>
@@ -15806,7 +15806,7 @@
       </c>
       <c r="I336" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>561068625</v>
+        <v>421795997</v>
       </c>
       <c r="J336" s="1">
         <v>10</v>
@@ -15848,7 +15848,7 @@
       </c>
       <c r="I337" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>342970281</v>
+        <v>53539403</v>
       </c>
       <c r="J337" s="1">
         <v>10</v>
@@ -15890,7 +15890,7 @@
       </c>
       <c r="I338" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>869392670</v>
+        <v>578071647</v>
       </c>
       <c r="J338" s="1">
         <v>10</v>
@@ -15932,7 +15932,7 @@
       </c>
       <c r="I339" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>901172661</v>
+        <v>671717681</v>
       </c>
       <c r="J339" s="1">
         <v>10</v>
@@ -15980,7 +15980,7 @@
       </c>
       <c r="I340" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>423906122</v>
+        <v>160926835</v>
       </c>
       <c r="J340" s="1">
         <v>10</v>
@@ -16022,7 +16022,7 @@
       </c>
       <c r="I341" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>628110973</v>
+        <v>712142454</v>
       </c>
       <c r="J341" s="1">
         <v>10</v>
@@ -16064,7 +16064,7 @@
       </c>
       <c r="I342" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>476490163</v>
+        <v>239353256</v>
       </c>
       <c r="J342" s="1">
         <v>10</v>
@@ -16106,7 +16106,7 @@
       </c>
       <c r="I343" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>895476591</v>
+        <v>274099468</v>
       </c>
       <c r="J343" s="1">
         <v>10</v>
@@ -16148,7 +16148,7 @@
       </c>
       <c r="I344" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>886373723</v>
+        <v>342062439</v>
       </c>
       <c r="J344" s="1">
         <v>10</v>
@@ -16193,7 +16193,7 @@
       </c>
       <c r="I345" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>305805779</v>
+        <v>689747997</v>
       </c>
       <c r="J345" s="1">
         <v>10</v>
@@ -16235,7 +16235,7 @@
       </c>
       <c r="I346" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>922275693</v>
+        <v>848398533</v>
       </c>
       <c r="J346" s="1">
         <v>10</v>
@@ -16277,7 +16277,7 @@
       </c>
       <c r="I347" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>568081144</v>
+        <v>965321087</v>
       </c>
       <c r="J347" s="1">
         <v>10</v>
@@ -16319,7 +16319,7 @@
       </c>
       <c r="I348" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>380195437</v>
+        <v>63464899</v>
       </c>
       <c r="J348" s="1">
         <v>10</v>
@@ -16361,7 +16361,7 @@
       </c>
       <c r="I349" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>587309734</v>
+        <v>482469077</v>
       </c>
       <c r="J349" s="1">
         <v>10</v>
@@ -16403,7 +16403,7 @@
       </c>
       <c r="I350" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>607349213</v>
+        <v>986384880</v>
       </c>
       <c r="J350" s="1">
         <v>10</v>
@@ -16448,7 +16448,7 @@
       </c>
       <c r="I351" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>634768098</v>
+        <v>267682009</v>
       </c>
       <c r="J351" s="1">
         <v>10</v>
@@ -16490,7 +16490,7 @@
       </c>
       <c r="I352" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>17135810</v>
+        <v>597701111</v>
       </c>
       <c r="J352" s="1">
         <v>10</v>
@@ -16532,7 +16532,7 @@
       </c>
       <c r="I353" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>943961105</v>
+        <v>659043862</v>
       </c>
       <c r="J353" s="1">
         <v>10</v>
@@ -16574,7 +16574,7 @@
       </c>
       <c r="I354" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>864310363</v>
+        <v>661834386</v>
       </c>
       <c r="J354" s="1">
         <v>10</v>
@@ -16619,7 +16619,7 @@
       </c>
       <c r="I355" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>544784127</v>
+        <v>521038791</v>
       </c>
       <c r="J355" s="1">
         <v>10</v>
@@ -16661,7 +16661,7 @@
       </c>
       <c r="I356" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>670314309</v>
+        <v>536246833</v>
       </c>
       <c r="J356" s="1">
         <v>10</v>
@@ -16703,7 +16703,7 @@
       </c>
       <c r="I357" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>428395368</v>
+        <v>848008493</v>
       </c>
       <c r="J357" s="1">
         <v>10</v>
@@ -16745,7 +16745,7 @@
       </c>
       <c r="I358" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>892050025</v>
+        <v>67155249</v>
       </c>
       <c r="J358" s="1">
         <v>10</v>
@@ -16787,7 +16787,7 @@
       </c>
       <c r="I359" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>169939295</v>
+        <v>346733910</v>
       </c>
       <c r="J359" s="1">
         <v>10</v>
@@ -16835,7 +16835,7 @@
       </c>
       <c r="I360" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>815949204</v>
+        <v>609109093</v>
       </c>
       <c r="J360" s="1">
         <v>10</v>
@@ -16877,7 +16877,7 @@
       </c>
       <c r="I361" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>747439353</v>
+        <v>450669304</v>
       </c>
       <c r="J361" s="1">
         <v>10</v>
@@ -16919,7 +16919,7 @@
       </c>
       <c r="I362" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>707841905</v>
+        <v>221142600</v>
       </c>
       <c r="J362" s="1">
         <v>10</v>
@@ -16961,7 +16961,7 @@
       </c>
       <c r="I363" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>88693525</v>
+        <v>495260996</v>
       </c>
       <c r="J363" s="1">
         <v>10</v>

</xml_diff>

<commit_message>
wip: changed firms/users seed (#212)
* wip: changed firms/users seed

* wip: changed seed for events
</commit_message>
<xml_diff>
--- a/graphql/db/events.xlsx
+++ b/graphql/db/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A74905-64BF-1D4A-92B8-1B3181524669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F9CDA6-F72C-1941-A338-54A2313A703F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="4240" windowWidth="36880" windowHeight="23500" xr2:uid="{E724A02B-0613-6046-AB06-036B70DCFCC0}"/>
+    <workbookView xWindow="12220" yWindow="5840" windowWidth="36880" windowHeight="23500" xr2:uid="{E724A02B-0613-6046-AB06-036B70DCFCC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE1BE4E-41DA-D14E-BD6A-74D507CD06A8}">
   <dimension ref="A1:O363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
-      <selection activeCell="D363" sqref="D363"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">RANDBETWEEN(10000, 999999999)</f>
-        <v>625331540</v>
+        <v>121775653</v>
       </c>
       <c r="J2" s="1">
         <v>10</v>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I66" ca="1" si="0">RANDBETWEEN(10000, 999999999)</f>
-        <v>30751941</v>
+        <v>712639313</v>
       </c>
       <c r="J3" s="1">
         <v>10</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>809945577</v>
+        <v>16572122</v>
       </c>
       <c r="J4" s="1">
         <v>10</v>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>273716082</v>
+        <v>499167949</v>
       </c>
       <c r="J5" s="1">
         <v>10</v>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>450029226</v>
+        <v>382438081</v>
       </c>
       <c r="J6" s="1">
         <v>10</v>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>600493946</v>
+        <v>16866156</v>
       </c>
       <c r="J7" s="1">
         <v>10</v>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>41083556</v>
+        <v>166811606</v>
       </c>
       <c r="J8" s="1">
         <v>10</v>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>743168612</v>
+        <v>171681057</v>
       </c>
       <c r="J9" s="1">
         <v>10</v>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>507126013</v>
+        <v>861908589</v>
       </c>
       <c r="J10" s="1">
         <v>10</v>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>679435351</v>
+        <v>679160087</v>
       </c>
       <c r="J11" s="1">
         <v>10</v>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>672480157</v>
+        <v>799138825</v>
       </c>
       <c r="J12" s="1">
         <v>10</v>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>870685116</v>
+        <v>827650866</v>
       </c>
       <c r="J13" s="1">
         <v>10</v>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>940813936</v>
+        <v>944129105</v>
       </c>
       <c r="J14" s="1">
         <v>10</v>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>898450770</v>
+        <v>562422811</v>
       </c>
       <c r="J15" s="1">
         <v>10</v>
@@ -2114,7 +2114,7 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>160167894</v>
+        <v>837549753</v>
       </c>
       <c r="J16" s="1">
         <v>10</v>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>294267594</v>
+        <v>555711927</v>
       </c>
       <c r="J17" s="1">
         <v>10</v>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>645512862</v>
+        <v>97961257</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>206513955</v>
+        <v>898702149</v>
       </c>
       <c r="J19" s="1">
         <v>10</v>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>480817336</v>
+        <v>716822292</v>
       </c>
       <c r="J20" s="1">
         <v>10</v>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="I21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>221135986</v>
+        <v>313457969</v>
       </c>
       <c r="J21" s="1">
         <v>10</v>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>179214977</v>
+        <v>234468338</v>
       </c>
       <c r="J22" s="1">
         <v>10</v>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>215855498</v>
+        <v>358522147</v>
       </c>
       <c r="J23" s="1">
         <v>10</v>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>507704743</v>
+        <v>467149079</v>
       </c>
       <c r="J24" s="1">
         <v>10</v>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>253745568</v>
+        <v>34911367</v>
       </c>
       <c r="J25" s="1">
         <v>10</v>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>79978683</v>
+        <v>28507764</v>
       </c>
       <c r="J26" s="1">
         <v>10</v>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="I27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>206342354</v>
+        <v>872755870</v>
       </c>
       <c r="J27" s="1">
         <v>10</v>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="I28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>987772960</v>
+        <v>11525812</v>
       </c>
       <c r="J28" s="1">
         <v>10</v>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="I29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3799461</v>
+        <v>729493490</v>
       </c>
       <c r="J29" s="1">
         <v>10</v>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="I30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>900936619</v>
+        <v>815220135</v>
       </c>
       <c r="J30" s="1">
         <v>10</v>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>490236409</v>
+        <v>461204293</v>
       </c>
       <c r="J31" s="1">
         <v>10</v>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>812705650</v>
+        <v>998334968</v>
       </c>
       <c r="J32" s="1">
         <v>10</v>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="I33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2043392</v>
+        <v>638462267</v>
       </c>
       <c r="J33" s="1">
         <v>10</v>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>345458951</v>
+        <v>331589032</v>
       </c>
       <c r="J34" s="1">
         <v>10</v>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="I35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>254337194</v>
+        <v>272327835</v>
       </c>
       <c r="J35" s="1">
         <v>10</v>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="I36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>850878419</v>
+        <v>621450918</v>
       </c>
       <c r="J36" s="1">
         <v>10</v>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="I37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>102194926</v>
+        <v>609084014</v>
       </c>
       <c r="J37" s="1">
         <v>10</v>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="I38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>582356511</v>
+        <v>522473943</v>
       </c>
       <c r="J38" s="1">
         <v>10</v>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="I39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>976587440</v>
+        <v>201354654</v>
       </c>
       <c r="J39" s="1">
         <v>10</v>
@@ -3143,7 +3143,7 @@
       </c>
       <c r="I40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>340777076</v>
+        <v>457344222</v>
       </c>
       <c r="J40" s="1">
         <v>10</v>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="I41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>694469522</v>
+        <v>497135078</v>
       </c>
       <c r="J41" s="1">
         <v>10</v>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="I42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>714940225</v>
+        <v>857017730</v>
       </c>
       <c r="J42" s="1">
         <v>10</v>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="I43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>322041168</v>
+        <v>762526902</v>
       </c>
       <c r="J43" s="1">
         <v>10</v>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="I44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>787489256</v>
+        <v>844444056</v>
       </c>
       <c r="J44" s="1">
         <v>10</v>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="I45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>886399247</v>
+        <v>399453277</v>
       </c>
       <c r="J45" s="1">
         <v>10</v>
@@ -3398,7 +3398,7 @@
       </c>
       <c r="I46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>968158827</v>
+        <v>895611349</v>
       </c>
       <c r="J46" s="1">
         <v>10</v>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="I47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>480097086</v>
+        <v>45834290</v>
       </c>
       <c r="J47" s="1">
         <v>10</v>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="I48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>968725436</v>
+        <v>478286887</v>
       </c>
       <c r="J48" s="1">
         <v>10</v>
@@ -3527,7 +3527,7 @@
       </c>
       <c r="I49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>168342868</v>
+        <v>732602838</v>
       </c>
       <c r="J49" s="1">
         <v>10</v>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="I50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>971024497</v>
+        <v>156814695</v>
       </c>
       <c r="J50" s="1">
         <v>10</v>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="I51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>895561231</v>
+        <v>709759611</v>
       </c>
       <c r="J51" s="1">
         <v>10</v>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="I52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>670190017</v>
+        <v>882443907</v>
       </c>
       <c r="J52" s="1">
         <v>10</v>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="I53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>214530231</v>
+        <v>521477089</v>
       </c>
       <c r="J53" s="1">
         <v>10</v>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="I54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>525009786</v>
+        <v>346077147</v>
       </c>
       <c r="J54" s="1">
         <v>10</v>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="I55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>182599138</v>
+        <v>805360981</v>
       </c>
       <c r="J55" s="1">
         <v>10</v>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="I56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>905874300</v>
+        <v>555074378</v>
       </c>
       <c r="J56" s="1">
         <v>10</v>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="I57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>456580857</v>
+        <v>446789667</v>
       </c>
       <c r="J57" s="1">
         <v>10</v>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="I58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>629495136</v>
+        <v>72641372</v>
       </c>
       <c r="J58" s="1">
         <v>10</v>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="I59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>23073038</v>
+        <v>443980505</v>
       </c>
       <c r="J59" s="1">
         <v>10</v>
@@ -3998,7 +3998,7 @@
       </c>
       <c r="I60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>889441872</v>
+        <v>213077318</v>
       </c>
       <c r="J60" s="1">
         <v>10</v>
@@ -4040,7 +4040,7 @@
       </c>
       <c r="I61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>789984656</v>
+        <v>202696099</v>
       </c>
       <c r="J61" s="1">
         <v>10</v>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="I62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>212242629</v>
+        <v>514673278</v>
       </c>
       <c r="J62" s="1">
         <v>10</v>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="I63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>144557243</v>
+        <v>139708597</v>
       </c>
       <c r="J63" s="1">
         <v>10</v>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="I64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>768581852</v>
+        <v>487080006</v>
       </c>
       <c r="J64" s="1">
         <v>10</v>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="I65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>543033277</v>
+        <v>574737036</v>
       </c>
       <c r="J65" s="1">
         <v>10</v>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="I66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>736840908</v>
+        <v>812772915</v>
       </c>
       <c r="J66" s="1">
         <v>10</v>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="I67" s="1">
         <f t="shared" ref="I67:I130" ca="1" si="1">RANDBETWEEN(10000, 999999999)</f>
-        <v>207546165</v>
+        <v>222669337</v>
       </c>
       <c r="J67" s="1">
         <v>10</v>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="I68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>895318681</v>
+        <v>713547083</v>
       </c>
       <c r="J68" s="1">
         <v>10</v>
@@ -4382,7 +4382,7 @@
       </c>
       <c r="I69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>327620465</v>
+        <v>406782853</v>
       </c>
       <c r="J69" s="1">
         <v>10</v>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="I70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>795803220</v>
+        <v>77283303</v>
       </c>
       <c r="J70" s="1">
         <v>10</v>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="I71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>17434278</v>
+        <v>847134617</v>
       </c>
       <c r="J71" s="1">
         <v>10</v>
@@ -4508,7 +4508,7 @@
       </c>
       <c r="I72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>547891383</v>
+        <v>964910038</v>
       </c>
       <c r="J72" s="1">
         <v>10</v>
@@ -4553,7 +4553,7 @@
       </c>
       <c r="I73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>705363431</v>
+        <v>638692113</v>
       </c>
       <c r="J73" s="1">
         <v>10</v>
@@ -4595,7 +4595,7 @@
       </c>
       <c r="I74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>15758164</v>
+        <v>466216070</v>
       </c>
       <c r="J74" s="1">
         <v>10</v>
@@ -4637,7 +4637,7 @@
       </c>
       <c r="I75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>285868334</v>
+        <v>641331748</v>
       </c>
       <c r="J75" s="1">
         <v>10</v>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="I76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>289860951</v>
+        <v>393268863</v>
       </c>
       <c r="J76" s="1">
         <v>10</v>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="I77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>412441752</v>
+        <v>145252197</v>
       </c>
       <c r="J77" s="1">
         <v>10</v>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="I78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>568415421</v>
+        <v>684025122</v>
       </c>
       <c r="J78" s="1">
         <v>10</v>
@@ -4811,7 +4811,7 @@
       </c>
       <c r="I79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>888526642</v>
+        <v>403016607</v>
       </c>
       <c r="J79" s="1">
         <v>10</v>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="I80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>442194917</v>
+        <v>288135862</v>
       </c>
       <c r="J80" s="1">
         <v>10</v>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="I81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>758928846</v>
+        <v>89858026</v>
       </c>
       <c r="J81" s="1">
         <v>10</v>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="I82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>422412059</v>
+        <v>180032652</v>
       </c>
       <c r="J82" s="1">
         <v>10</v>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="I83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>834979789</v>
+        <v>118814403</v>
       </c>
       <c r="J83" s="1">
         <v>10</v>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="I84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>981375192</v>
+        <v>553185327</v>
       </c>
       <c r="J84" s="1">
         <v>10</v>
@@ -5066,7 +5066,7 @@
       </c>
       <c r="I85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>722668259</v>
+        <v>939461555</v>
       </c>
       <c r="J85" s="1">
         <v>10</v>
@@ -5108,7 +5108,7 @@
       </c>
       <c r="I86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>289386993</v>
+        <v>701131355</v>
       </c>
       <c r="J86" s="1">
         <v>10</v>
@@ -5150,7 +5150,7 @@
       </c>
       <c r="I87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>267454391</v>
+        <v>892876419</v>
       </c>
       <c r="J87" s="1">
         <v>10</v>
@@ -5192,7 +5192,7 @@
       </c>
       <c r="I88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>19422213</v>
+        <v>522934058</v>
       </c>
       <c r="J88" s="1">
         <v>10</v>
@@ -5237,7 +5237,7 @@
       </c>
       <c r="I89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>399744229</v>
+        <v>94113747</v>
       </c>
       <c r="J89" s="1">
         <v>10</v>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="I90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>46092920</v>
+        <v>45984708</v>
       </c>
       <c r="J90" s="1">
         <v>10</v>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="I91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>902450963</v>
+        <v>240483775</v>
       </c>
       <c r="J91" s="1">
         <v>10</v>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="I92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>102738191</v>
+        <v>657246837</v>
       </c>
       <c r="J92" s="1">
         <v>10</v>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="I93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>641009909</v>
+        <v>452650124</v>
       </c>
       <c r="J93" s="1">
         <v>10</v>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="I94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>883191100</v>
+        <v>507560916</v>
       </c>
       <c r="J94" s="1">
         <v>10</v>
@@ -5492,7 +5492,7 @@
       </c>
       <c r="I95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>898431312</v>
+        <v>493483729</v>
       </c>
       <c r="J95" s="1">
         <v>10</v>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="I96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>427926908</v>
+        <v>734197782</v>
       </c>
       <c r="J96" s="1">
         <v>10</v>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="I97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>895841683</v>
+        <v>200686733</v>
       </c>
       <c r="J97" s="1">
         <v>10</v>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="I98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>159441286</v>
+        <v>15711510</v>
       </c>
       <c r="J98" s="1">
         <v>10</v>
@@ -5666,7 +5666,7 @@
       </c>
       <c r="I99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>255393321</v>
+        <v>33676816</v>
       </c>
       <c r="J99" s="1">
         <v>10</v>
@@ -5708,7 +5708,7 @@
       </c>
       <c r="I100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>906660297</v>
+        <v>69005753</v>
       </c>
       <c r="J100" s="1">
         <v>10</v>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="I101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>313841732</v>
+        <v>337506105</v>
       </c>
       <c r="J101" s="1">
         <v>10</v>
@@ -5792,7 +5792,7 @@
       </c>
       <c r="I102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>547601894</v>
+        <v>132311435</v>
       </c>
       <c r="J102" s="1">
         <v>10</v>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="I103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>514375790</v>
+        <v>105461003</v>
       </c>
       <c r="J103" s="1">
         <v>10</v>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="I104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>229673797</v>
+        <v>366852788</v>
       </c>
       <c r="J104" s="1">
         <v>10</v>
@@ -5921,7 +5921,7 @@
       </c>
       <c r="I105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>202909326</v>
+        <v>979668662</v>
       </c>
       <c r="J105" s="1">
         <v>10</v>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="I106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>498505261</v>
+        <v>368181240</v>
       </c>
       <c r="J106" s="1">
         <v>10</v>
@@ -6005,7 +6005,7 @@
       </c>
       <c r="I107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>372957562</v>
+        <v>569877319</v>
       </c>
       <c r="J107" s="1">
         <v>10</v>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="I108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>768855842</v>
+        <v>950109160</v>
       </c>
       <c r="J108" s="1">
         <v>10</v>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="I109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>61152844</v>
+        <v>490270569</v>
       </c>
       <c r="J109" s="1">
         <v>10</v>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="I110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>713581603</v>
+        <v>609723466</v>
       </c>
       <c r="J110" s="1">
         <v>10</v>
@@ -6176,7 +6176,7 @@
       </c>
       <c r="I111" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>989831777</v>
+        <v>992907997</v>
       </c>
       <c r="J111" s="1">
         <v>10</v>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="I112" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>145158918</v>
+        <v>740575</v>
       </c>
       <c r="J112" s="1">
         <v>10</v>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="I113" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>885487508</v>
+        <v>747128782</v>
       </c>
       <c r="J113" s="1">
         <v>10</v>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="I114" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>566704245</v>
+        <v>642983311</v>
       </c>
       <c r="J114" s="1">
         <v>10</v>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="I115" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>24838487</v>
+        <v>125837685</v>
       </c>
       <c r="J115" s="1">
         <v>10</v>
@@ -6389,7 +6389,7 @@
       </c>
       <c r="I116" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>286002585</v>
+        <v>633239549</v>
       </c>
       <c r="J116" s="1">
         <v>10</v>
@@ -6431,7 +6431,7 @@
       </c>
       <c r="I117" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>274725884</v>
+        <v>361636177</v>
       </c>
       <c r="J117" s="1">
         <v>10</v>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="I118" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>288447827</v>
+        <v>814755204</v>
       </c>
       <c r="J118" s="1">
         <v>10</v>
@@ -6521,7 +6521,7 @@
       </c>
       <c r="I119" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>412474613</v>
+        <v>883357217</v>
       </c>
       <c r="J119" s="1">
         <v>10</v>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="I120" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>923884427</v>
+        <v>82780912</v>
       </c>
       <c r="J120" s="1">
         <v>10</v>
@@ -6605,7 +6605,7 @@
       </c>
       <c r="I121" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>559692358</v>
+        <v>605233158</v>
       </c>
       <c r="J121" s="1">
         <v>10</v>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="I122" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>822440947</v>
+        <v>505706160</v>
       </c>
       <c r="J122" s="1" t="s">
         <v>9</v>
@@ -6695,7 +6695,7 @@
       </c>
       <c r="I123" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>236869139</v>
+        <v>736065542</v>
       </c>
       <c r="J123" s="1">
         <v>10</v>
@@ -6740,7 +6740,7 @@
       </c>
       <c r="I124" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>33726421</v>
+        <v>383624783</v>
       </c>
       <c r="J124" s="1">
         <v>10</v>
@@ -6782,7 +6782,7 @@
       </c>
       <c r="I125" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>898893407</v>
+        <v>862350601</v>
       </c>
       <c r="J125" s="1">
         <v>10</v>
@@ -6824,7 +6824,7 @@
       </c>
       <c r="I126" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>44422427</v>
+        <v>105021027</v>
       </c>
       <c r="J126" s="1">
         <v>10</v>
@@ -6866,7 +6866,7 @@
       </c>
       <c r="I127" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>236145228</v>
+        <v>81494586</v>
       </c>
       <c r="J127" s="1">
         <v>10</v>
@@ -6908,7 +6908,7 @@
       </c>
       <c r="I128" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>633212729</v>
+        <v>841406877</v>
       </c>
       <c r="J128" s="1">
         <v>10</v>
@@ -6950,7 +6950,7 @@
       </c>
       <c r="I129" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>76651192</v>
+        <v>460331503</v>
       </c>
       <c r="J129" s="1">
         <v>10</v>
@@ -6995,7 +6995,7 @@
       </c>
       <c r="I130" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>385810698</v>
+        <v>815718416</v>
       </c>
       <c r="J130" s="1">
         <v>10</v>
@@ -7037,7 +7037,7 @@
       </c>
       <c r="I131" s="1">
         <f t="shared" ref="I131:I194" ca="1" si="2">RANDBETWEEN(10000, 999999999)</f>
-        <v>47932353</v>
+        <v>120936844</v>
       </c>
       <c r="J131" s="1">
         <v>10</v>
@@ -7079,7 +7079,7 @@
       </c>
       <c r="I132" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>293056477</v>
+        <v>750642237</v>
       </c>
       <c r="J132" s="1">
         <v>10</v>
@@ -7121,7 +7121,7 @@
       </c>
       <c r="I133" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>363143147</v>
+        <v>142721654</v>
       </c>
       <c r="J133" s="1">
         <v>10</v>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="I134" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>141353942</v>
+        <v>672781834</v>
       </c>
       <c r="J134" s="1">
         <v>10</v>
@@ -7208,7 +7208,7 @@
       </c>
       <c r="I135" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>144857299</v>
+        <v>749666677</v>
       </c>
       <c r="J135" s="1">
         <v>10</v>
@@ -7250,7 +7250,7 @@
       </c>
       <c r="I136" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>921178563</v>
+        <v>757884608</v>
       </c>
       <c r="J136" s="1">
         <v>10</v>
@@ -7292,7 +7292,7 @@
       </c>
       <c r="I137" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>114758562</v>
+        <v>939091921</v>
       </c>
       <c r="J137" s="1">
         <v>10</v>
@@ -7334,7 +7334,7 @@
       </c>
       <c r="I138" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>943048865</v>
+        <v>328882294</v>
       </c>
       <c r="J138" s="1">
         <v>10</v>
@@ -7382,7 +7382,7 @@
       </c>
       <c r="I139" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>872284708</v>
+        <v>44949736</v>
       </c>
       <c r="J139" s="1">
         <v>10</v>
@@ -7424,7 +7424,7 @@
       </c>
       <c r="I140" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>266419514</v>
+        <v>362090387</v>
       </c>
       <c r="J140" s="1">
         <v>10</v>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="I141" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>16448185</v>
+        <v>791067193</v>
       </c>
       <c r="J141" s="1">
         <v>10</v>
@@ -7508,7 +7508,7 @@
       </c>
       <c r="I142" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>827469724</v>
+        <v>407188729</v>
       </c>
       <c r="J142" s="1">
         <v>10</v>
@@ -7550,7 +7550,7 @@
       </c>
       <c r="I143" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>993604029</v>
+        <v>802622797</v>
       </c>
       <c r="J143" s="1">
         <v>10</v>
@@ -7595,7 +7595,7 @@
       </c>
       <c r="I144" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>419897957</v>
+        <v>311157288</v>
       </c>
       <c r="J144" s="1">
         <v>10</v>
@@ -7637,7 +7637,7 @@
       </c>
       <c r="I145" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>25275797</v>
+        <v>148440576</v>
       </c>
       <c r="J145" s="1">
         <v>10</v>
@@ -7679,7 +7679,7 @@
       </c>
       <c r="I146" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>417205696</v>
+        <v>997265996</v>
       </c>
       <c r="J146" s="1">
         <v>10</v>
@@ -7721,7 +7721,7 @@
       </c>
       <c r="I147" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>745521558</v>
+        <v>783619519</v>
       </c>
       <c r="J147" s="1">
         <v>10</v>
@@ -7763,7 +7763,7 @@
       </c>
       <c r="I148" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>390611576</v>
+        <v>647544992</v>
       </c>
       <c r="J148" s="1">
         <v>10</v>
@@ -7805,7 +7805,7 @@
       </c>
       <c r="I149" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>110179296</v>
+        <v>676257196</v>
       </c>
       <c r="J149" s="1">
         <v>10</v>
@@ -7850,7 +7850,7 @@
       </c>
       <c r="I150" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>80796791</v>
+        <v>663373617</v>
       </c>
       <c r="J150" s="1">
         <v>10</v>
@@ -7892,7 +7892,7 @@
       </c>
       <c r="I151" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>118458358</v>
+        <v>921835429</v>
       </c>
       <c r="J151" s="1">
         <v>10</v>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="I152" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>322959240</v>
+        <v>915333310</v>
       </c>
       <c r="J152" s="1">
         <v>10</v>
@@ -7976,7 +7976,7 @@
       </c>
       <c r="I153" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>815367574</v>
+        <v>513283400</v>
       </c>
       <c r="J153" s="1">
         <v>10</v>
@@ -8021,7 +8021,7 @@
       </c>
       <c r="I154" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>638840997</v>
+        <v>914771421</v>
       </c>
       <c r="J154" s="1">
         <v>10</v>
@@ -8063,7 +8063,7 @@
       </c>
       <c r="I155" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>401662825</v>
+        <v>908945747</v>
       </c>
       <c r="J155" s="1">
         <v>10</v>
@@ -8105,7 +8105,7 @@
       </c>
       <c r="I156" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>261303508</v>
+        <v>694168536</v>
       </c>
       <c r="J156" s="1">
         <v>10</v>
@@ -8147,7 +8147,7 @@
       </c>
       <c r="I157" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>839903401</v>
+        <v>136440553</v>
       </c>
       <c r="J157" s="1">
         <v>10</v>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="I158" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>494950985</v>
+        <v>619720802</v>
       </c>
       <c r="J158" s="1">
         <v>10</v>
@@ -8237,7 +8237,7 @@
       </c>
       <c r="I159" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>675400652</v>
+        <v>980567024</v>
       </c>
       <c r="J159" s="1">
         <v>10</v>
@@ -8279,7 +8279,7 @@
       </c>
       <c r="I160" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>996174350</v>
+        <v>155444710</v>
       </c>
       <c r="J160" s="1">
         <v>10</v>
@@ -8321,7 +8321,7 @@
       </c>
       <c r="I161" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>805548045</v>
+        <v>105757679</v>
       </c>
       <c r="J161" s="1">
         <v>10</v>
@@ -8363,7 +8363,7 @@
       </c>
       <c r="I162" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>393341297</v>
+        <v>453976269</v>
       </c>
       <c r="J162" s="1">
         <v>10</v>
@@ -8405,7 +8405,7 @@
       </c>
       <c r="I163" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>679815980</v>
+        <v>282591947</v>
       </c>
       <c r="J163" s="1">
         <v>10</v>
@@ -8450,7 +8450,7 @@
       </c>
       <c r="I164" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>180427492</v>
+        <v>377098486</v>
       </c>
       <c r="J164" s="1">
         <v>10</v>
@@ -8492,7 +8492,7 @@
       </c>
       <c r="I165" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>727173325</v>
+        <v>41222685</v>
       </c>
       <c r="J165" s="1">
         <v>10</v>
@@ -8534,7 +8534,7 @@
       </c>
       <c r="I166" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>292170908</v>
+        <v>932115984</v>
       </c>
       <c r="J166" s="1">
         <v>10</v>
@@ -8576,7 +8576,7 @@
       </c>
       <c r="I167" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>846203375</v>
+        <v>228133459</v>
       </c>
       <c r="J167" s="1">
         <v>10</v>
@@ -8618,7 +8618,7 @@
       </c>
       <c r="I168" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>758444416</v>
+        <v>631137297</v>
       </c>
       <c r="J168" s="1">
         <v>10</v>
@@ -8660,7 +8660,7 @@
       </c>
       <c r="I169" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>51681408</v>
+        <v>88524107</v>
       </c>
       <c r="J169" s="1">
         <v>10</v>
@@ -8705,7 +8705,7 @@
       </c>
       <c r="I170" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>976259301</v>
+        <v>110553316</v>
       </c>
       <c r="J170" s="1">
         <v>10</v>
@@ -8747,7 +8747,7 @@
       </c>
       <c r="I171" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>639487357</v>
+        <v>122246876</v>
       </c>
       <c r="J171" s="1">
         <v>10</v>
@@ -8789,7 +8789,7 @@
       </c>
       <c r="I172" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>376063135</v>
+        <v>661862583</v>
       </c>
       <c r="J172" s="1">
         <v>10</v>
@@ -8831,7 +8831,7 @@
       </c>
       <c r="I173" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>643537201</v>
+        <v>116099191</v>
       </c>
       <c r="J173" s="1">
         <v>10</v>
@@ -8876,7 +8876,7 @@
       </c>
       <c r="I174" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>118705106</v>
+        <v>223152634</v>
       </c>
       <c r="J174" s="1">
         <v>10</v>
@@ -8918,7 +8918,7 @@
       </c>
       <c r="I175" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>558943061</v>
+        <v>348717993</v>
       </c>
       <c r="J175" s="1">
         <v>10</v>
@@ -8960,7 +8960,7 @@
       </c>
       <c r="I176" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>120013876</v>
+        <v>334559890</v>
       </c>
       <c r="J176" s="1">
         <v>10</v>
@@ -9002,7 +9002,7 @@
       </c>
       <c r="I177" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>215894838</v>
+        <v>251364590</v>
       </c>
       <c r="J177" s="1">
         <v>10</v>
@@ -9044,7 +9044,7 @@
       </c>
       <c r="I178" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>58976211</v>
+        <v>601601931</v>
       </c>
       <c r="J178" s="1">
         <v>10</v>
@@ -9092,7 +9092,7 @@
       </c>
       <c r="I179" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>586276035</v>
+        <v>790045853</v>
       </c>
       <c r="J179" s="1">
         <v>10</v>
@@ -9134,7 +9134,7 @@
       </c>
       <c r="I180" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>492041997</v>
+        <v>402287434</v>
       </c>
       <c r="J180" s="1">
         <v>10</v>
@@ -9176,7 +9176,7 @@
       </c>
       <c r="I181" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>387660918</v>
+        <v>436986178</v>
       </c>
       <c r="J181" s="1">
         <v>10</v>
@@ -9218,7 +9218,7 @@
       </c>
       <c r="I182" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>892476495</v>
+        <v>143141681</v>
       </c>
       <c r="J182" s="1">
         <v>10</v>
@@ -9260,7 +9260,7 @@
       </c>
       <c r="I183" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>81588147</v>
+        <v>806340374</v>
       </c>
       <c r="J183" s="1">
         <v>10</v>
@@ -9305,7 +9305,7 @@
       </c>
       <c r="I184" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>195090741</v>
+        <v>25144739</v>
       </c>
       <c r="J184" s="1">
         <v>10</v>
@@ -9347,7 +9347,7 @@
       </c>
       <c r="I185" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>841423113</v>
+        <v>414654109</v>
       </c>
       <c r="J185" s="1">
         <v>10</v>
@@ -9389,7 +9389,7 @@
       </c>
       <c r="I186" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>207086794</v>
+        <v>921693651</v>
       </c>
       <c r="J186" s="1">
         <v>10</v>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="I187" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>267350424</v>
+        <v>272161768</v>
       </c>
       <c r="J187" s="1">
         <v>10</v>
@@ -9473,7 +9473,7 @@
       </c>
       <c r="I188" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>765035003</v>
+        <v>680306898</v>
       </c>
       <c r="J188" s="1">
         <v>10</v>
@@ -9515,7 +9515,7 @@
       </c>
       <c r="I189" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>135450279</v>
+        <v>781348434</v>
       </c>
       <c r="J189" s="1">
         <v>10</v>
@@ -9560,7 +9560,7 @@
       </c>
       <c r="I190" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>30764789</v>
+        <v>162741133</v>
       </c>
       <c r="J190" s="1">
         <v>10</v>
@@ -9602,7 +9602,7 @@
       </c>
       <c r="I191" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>816217469</v>
+        <v>208324202</v>
       </c>
       <c r="J191" s="1">
         <v>10</v>
@@ -9644,7 +9644,7 @@
       </c>
       <c r="I192" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>612132712</v>
+        <v>840548857</v>
       </c>
       <c r="J192" s="1">
         <v>10</v>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="I193" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>313014678</v>
+        <v>618960203</v>
       </c>
       <c r="J193" s="1">
         <v>10</v>
@@ -9731,7 +9731,7 @@
       </c>
       <c r="I194" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>535358395</v>
+        <v>913124220</v>
       </c>
       <c r="J194" s="1">
         <v>10</v>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="I195" s="1">
         <f t="shared" ref="I195:I258" ca="1" si="3">RANDBETWEEN(10000, 999999999)</f>
-        <v>397917150</v>
+        <v>781787376</v>
       </c>
       <c r="J195" s="1">
         <v>10</v>
@@ -9815,7 +9815,7 @@
       </c>
       <c r="I196" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>648908145</v>
+        <v>340179644</v>
       </c>
       <c r="J196" s="1">
         <v>10</v>
@@ -9857,7 +9857,7 @@
       </c>
       <c r="I197" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>65346387</v>
+        <v>562591118</v>
       </c>
       <c r="J197" s="1">
         <v>10</v>
@@ -9899,7 +9899,7 @@
       </c>
       <c r="I198" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>277461883</v>
+        <v>636834140</v>
       </c>
       <c r="J198" s="1">
         <v>10</v>
@@ -9947,7 +9947,7 @@
       </c>
       <c r="I199" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>128877670</v>
+        <v>960712313</v>
       </c>
       <c r="J199" s="1">
         <v>10</v>
@@ -9989,7 +9989,7 @@
       </c>
       <c r="I200" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>963008941</v>
+        <v>509400072</v>
       </c>
       <c r="J200" s="1">
         <v>10</v>
@@ -10031,7 +10031,7 @@
       </c>
       <c r="I201" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>921269555</v>
+        <v>520917588</v>
       </c>
       <c r="J201" s="1">
         <v>10</v>
@@ -10073,7 +10073,7 @@
       </c>
       <c r="I202" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>729696945</v>
+        <v>627091076</v>
       </c>
       <c r="J202" s="1">
         <v>10</v>
@@ -10115,7 +10115,7 @@
       </c>
       <c r="I203" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>951576542</v>
+        <v>567235351</v>
       </c>
       <c r="J203" s="1">
         <v>10</v>
@@ -10160,7 +10160,7 @@
       </c>
       <c r="I204" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>489469983</v>
+        <v>792265721</v>
       </c>
       <c r="J204" s="1">
         <v>10</v>
@@ -10202,7 +10202,7 @@
       </c>
       <c r="I205" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>269308195</v>
+        <v>625320235</v>
       </c>
       <c r="J205" s="1">
         <v>10</v>
@@ -10244,7 +10244,7 @@
       </c>
       <c r="I206" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>269596710</v>
+        <v>238252839</v>
       </c>
       <c r="J206" s="1">
         <v>10</v>
@@ -10286,7 +10286,7 @@
       </c>
       <c r="I207" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>893543235</v>
+        <v>887083965</v>
       </c>
       <c r="J207" s="1">
         <v>10</v>
@@ -10328,7 +10328,7 @@
       </c>
       <c r="I208" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>873162938</v>
+        <v>180509369</v>
       </c>
       <c r="J208" s="1">
         <v>10</v>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="I209" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>852320958</v>
+        <v>707981957</v>
       </c>
       <c r="J209" s="1">
         <v>10</v>
@@ -10415,7 +10415,7 @@
       </c>
       <c r="I210" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>585205612</v>
+        <v>517506718</v>
       </c>
       <c r="J210" s="1">
         <v>10</v>
@@ -10457,7 +10457,7 @@
       </c>
       <c r="I211" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>593162227</v>
+        <v>34653413</v>
       </c>
       <c r="J211" s="1">
         <v>10</v>
@@ -10499,7 +10499,7 @@
       </c>
       <c r="I212" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>154335304</v>
+        <v>663911861</v>
       </c>
       <c r="J212" s="1">
         <v>10</v>
@@ -10541,7 +10541,7 @@
       </c>
       <c r="I213" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>314801014</v>
+        <v>359011380</v>
       </c>
       <c r="J213" s="1">
         <v>10</v>
@@ -10586,7 +10586,7 @@
       </c>
       <c r="I214" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>415987437</v>
+        <v>161118030</v>
       </c>
       <c r="J214" s="1">
         <v>10</v>
@@ -10628,7 +10628,7 @@
       </c>
       <c r="I215" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>562235478</v>
+        <v>426106916</v>
       </c>
       <c r="J215" s="1">
         <v>10</v>
@@ -10670,7 +10670,7 @@
       </c>
       <c r="I216" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>194301586</v>
+        <v>673455538</v>
       </c>
       <c r="J216" s="1">
         <v>10</v>
@@ -10712,7 +10712,7 @@
       </c>
       <c r="I217" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>57543367</v>
+        <v>910780741</v>
       </c>
       <c r="J217" s="1">
         <v>10</v>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="I218" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>246713722</v>
+        <v>868402780</v>
       </c>
       <c r="J218" s="1">
         <v>10</v>
@@ -10802,7 +10802,7 @@
       </c>
       <c r="I219" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>694949276</v>
+        <v>548700503</v>
       </c>
       <c r="J219" s="1">
         <v>10</v>
@@ -10844,7 +10844,7 @@
       </c>
       <c r="I220" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>298064284</v>
+        <v>82759777</v>
       </c>
       <c r="J220" s="1">
         <v>10</v>
@@ -10886,7 +10886,7 @@
       </c>
       <c r="I221" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>680075660</v>
+        <v>678016888</v>
       </c>
       <c r="J221" s="1">
         <v>10</v>
@@ -10928,7 +10928,7 @@
       </c>
       <c r="I222" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>614548009</v>
+        <v>733518561</v>
       </c>
       <c r="J222" s="1">
         <v>10</v>
@@ -10970,7 +10970,7 @@
       </c>
       <c r="I223" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>539306049</v>
+        <v>257837652</v>
       </c>
       <c r="J223" s="1">
         <v>10</v>
@@ -11015,7 +11015,7 @@
       </c>
       <c r="I224" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>129042654</v>
+        <v>914463031</v>
       </c>
       <c r="J224" s="1">
         <v>10</v>
@@ -11057,7 +11057,7 @@
       </c>
       <c r="I225" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>391435457</v>
+        <v>411668986</v>
       </c>
       <c r="J225" s="1">
         <v>10</v>
@@ -11099,7 +11099,7 @@
       </c>
       <c r="I226" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>806098885</v>
+        <v>193076304</v>
       </c>
       <c r="J226" s="1">
         <v>10</v>
@@ -11141,7 +11141,7 @@
       </c>
       <c r="I227" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>522939609</v>
+        <v>718779582</v>
       </c>
       <c r="J227" s="1">
         <v>10</v>
@@ -11183,7 +11183,7 @@
       </c>
       <c r="I228" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>344745825</v>
+        <v>203926146</v>
       </c>
       <c r="J228" s="1">
         <v>10</v>
@@ -11225,7 +11225,7 @@
       </c>
       <c r="I229" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>514828792</v>
+        <v>733339146</v>
       </c>
       <c r="J229" s="1">
         <v>10</v>
@@ -11270,7 +11270,7 @@
       </c>
       <c r="I230" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>929333286</v>
+        <v>51982535</v>
       </c>
       <c r="J230" s="1">
         <v>10</v>
@@ -11312,7 +11312,7 @@
       </c>
       <c r="I231" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>198195112</v>
+        <v>50585586</v>
       </c>
       <c r="J231" s="1">
         <v>10</v>
@@ -11354,7 +11354,7 @@
       </c>
       <c r="I232" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>952502234</v>
+        <v>216164571</v>
       </c>
       <c r="J232" s="1">
         <v>10</v>
@@ -11396,7 +11396,7 @@
       </c>
       <c r="I233" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>676141464</v>
+        <v>152820177</v>
       </c>
       <c r="J233" s="1">
         <v>10</v>
@@ -11441,7 +11441,7 @@
       </c>
       <c r="I234" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>450262616</v>
+        <v>327804652</v>
       </c>
       <c r="J234" s="1">
         <v>10</v>
@@ -11483,7 +11483,7 @@
       </c>
       <c r="I235" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>758408859</v>
+        <v>880550112</v>
       </c>
       <c r="J235" s="1">
         <v>10</v>
@@ -11525,7 +11525,7 @@
       </c>
       <c r="I236" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>183223399</v>
+        <v>416533483</v>
       </c>
       <c r="J236" s="1">
         <v>10</v>
@@ -11567,7 +11567,7 @@
       </c>
       <c r="I237" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>521483584</v>
+        <v>406273015</v>
       </c>
       <c r="J237" s="1">
         <v>10</v>
@@ -11609,7 +11609,7 @@
       </c>
       <c r="I238" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>708971753</v>
+        <v>647368304</v>
       </c>
       <c r="J238" s="1">
         <v>10</v>
@@ -11657,7 +11657,7 @@
       </c>
       <c r="I239" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>635012314</v>
+        <v>921136570</v>
       </c>
       <c r="J239" s="1">
         <v>10</v>
@@ -11699,7 +11699,7 @@
       </c>
       <c r="I240" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>375508774</v>
+        <v>466059559</v>
       </c>
       <c r="J240" s="1">
         <v>10</v>
@@ -11741,7 +11741,7 @@
       </c>
       <c r="I241" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>531002872</v>
+        <v>325214577</v>
       </c>
       <c r="J241" s="1">
         <v>10</v>
@@ -11783,7 +11783,7 @@
       </c>
       <c r="I242" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>690098173</v>
+        <v>799802118</v>
       </c>
       <c r="J242" s="1">
         <v>10</v>
@@ -11825,7 +11825,7 @@
       </c>
       <c r="I243" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>528393304</v>
+        <v>484813859</v>
       </c>
       <c r="J243" s="1" t="s">
         <v>9</v>
@@ -11873,7 +11873,7 @@
       </c>
       <c r="I244" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>834424761</v>
+        <v>405774722</v>
       </c>
       <c r="J244" s="1">
         <v>10</v>
@@ -11918,7 +11918,7 @@
       </c>
       <c r="I245" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>789670317</v>
+        <v>906036569</v>
       </c>
       <c r="J245" s="1">
         <v>10</v>
@@ -11960,7 +11960,7 @@
       </c>
       <c r="I246" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>774667783</v>
+        <v>731274972</v>
       </c>
       <c r="J246" s="1">
         <v>10</v>
@@ -12002,7 +12002,7 @@
       </c>
       <c r="I247" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>951231306</v>
+        <v>677869435</v>
       </c>
       <c r="J247" s="1">
         <v>10</v>
@@ -12044,7 +12044,7 @@
       </c>
       <c r="I248" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>779200389</v>
+        <v>675947841</v>
       </c>
       <c r="J248" s="1">
         <v>10</v>
@@ -12086,7 +12086,7 @@
       </c>
       <c r="I249" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>426459715</v>
+        <v>392462031</v>
       </c>
       <c r="J249" s="1">
         <v>10</v>
@@ -12128,7 +12128,7 @@
       </c>
       <c r="I250" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>583043984</v>
+        <v>256618930</v>
       </c>
       <c r="J250" s="1">
         <v>10</v>
@@ -12173,7 +12173,7 @@
       </c>
       <c r="I251" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>161995362</v>
+        <v>752976955</v>
       </c>
       <c r="J251" s="1">
         <v>10</v>
@@ -12215,7 +12215,7 @@
       </c>
       <c r="I252" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>855095107</v>
+        <v>289901443</v>
       </c>
       <c r="J252" s="1">
         <v>10</v>
@@ -12257,7 +12257,7 @@
       </c>
       <c r="I253" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>837608381</v>
+        <v>955759311</v>
       </c>
       <c r="J253" s="1">
         <v>10</v>
@@ -12299,7 +12299,7 @@
       </c>
       <c r="I254" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>503407974</v>
+        <v>523571071</v>
       </c>
       <c r="J254" s="1">
         <v>10</v>
@@ -12344,7 +12344,7 @@
       </c>
       <c r="I255" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>770900975</v>
+        <v>257235074</v>
       </c>
       <c r="J255" s="1">
         <v>10</v>
@@ -12386,7 +12386,7 @@
       </c>
       <c r="I256" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>863282704</v>
+        <v>111577062</v>
       </c>
       <c r="J256" s="1">
         <v>10</v>
@@ -12428,7 +12428,7 @@
       </c>
       <c r="I257" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>399761469</v>
+        <v>724301869</v>
       </c>
       <c r="J257" s="1">
         <v>10</v>
@@ -12470,7 +12470,7 @@
       </c>
       <c r="I258" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>542059458</v>
+        <v>98681242</v>
       </c>
       <c r="J258" s="1">
         <v>10</v>
@@ -12512,7 +12512,7 @@
       </c>
       <c r="I259" s="1">
         <f t="shared" ref="I259:I322" ca="1" si="4">RANDBETWEEN(10000, 999999999)</f>
-        <v>585123455</v>
+        <v>693201464</v>
       </c>
       <c r="J259" s="1">
         <v>10</v>
@@ -12560,7 +12560,7 @@
       </c>
       <c r="I260" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>430809491</v>
+        <v>189431570</v>
       </c>
       <c r="J260" s="1">
         <v>10</v>
@@ -12602,7 +12602,7 @@
       </c>
       <c r="I261" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>73206765</v>
+        <v>931225257</v>
       </c>
       <c r="J261" s="1">
         <v>10</v>
@@ -12644,7 +12644,7 @@
       </c>
       <c r="I262" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>117721817</v>
+        <v>693200515</v>
       </c>
       <c r="J262" s="1">
         <v>10</v>
@@ -12686,7 +12686,7 @@
       </c>
       <c r="I263" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>994017512</v>
+        <v>947405413</v>
       </c>
       <c r="J263" s="1">
         <v>10</v>
@@ -12728,7 +12728,7 @@
       </c>
       <c r="I264" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>29160037</v>
+        <v>431279751</v>
       </c>
       <c r="J264" s="1">
         <v>10</v>
@@ -12773,7 +12773,7 @@
       </c>
       <c r="I265" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>133245751</v>
+        <v>130131623</v>
       </c>
       <c r="J265" s="1">
         <v>10</v>
@@ -12815,7 +12815,7 @@
       </c>
       <c r="I266" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>996607580</v>
+        <v>547989221</v>
       </c>
       <c r="J266" s="1">
         <v>10</v>
@@ -12857,7 +12857,7 @@
       </c>
       <c r="I267" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>214591694</v>
+        <v>104394831</v>
       </c>
       <c r="J267" s="1">
         <v>10</v>
@@ -12899,7 +12899,7 @@
       </c>
       <c r="I268" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>780440707</v>
+        <v>386564089</v>
       </c>
       <c r="J268" s="1">
         <v>10</v>
@@ -12941,7 +12941,7 @@
       </c>
       <c r="I269" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>130460090</v>
+        <v>559237582</v>
       </c>
       <c r="J269" s="1">
         <v>10</v>
@@ -12983,7 +12983,7 @@
       </c>
       <c r="I270" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>586722756</v>
+        <v>888860437</v>
       </c>
       <c r="J270" s="1">
         <v>10</v>
@@ -13028,7 +13028,7 @@
       </c>
       <c r="I271" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>839503507</v>
+        <v>102186118</v>
       </c>
       <c r="J271" s="1">
         <v>10</v>
@@ -13070,7 +13070,7 @@
       </c>
       <c r="I272" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>394672460</v>
+        <v>536970915</v>
       </c>
       <c r="J272" s="1">
         <v>10</v>
@@ -13112,7 +13112,7 @@
       </c>
       <c r="I273" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1239305</v>
+        <v>458441055</v>
       </c>
       <c r="J273" s="1">
         <v>10</v>
@@ -13154,7 +13154,7 @@
       </c>
       <c r="I274" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>194946347</v>
+        <v>890301937</v>
       </c>
       <c r="J274" s="1">
         <v>10</v>
@@ -13199,7 +13199,7 @@
       </c>
       <c r="I275" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>338416324</v>
+        <v>833138445</v>
       </c>
       <c r="J275" s="1">
         <v>10</v>
@@ -13241,7 +13241,7 @@
       </c>
       <c r="I276" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>385386257</v>
+        <v>769771259</v>
       </c>
       <c r="J276" s="1">
         <v>10</v>
@@ -13283,7 +13283,7 @@
       </c>
       <c r="I277" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>49583594</v>
+        <v>183870421</v>
       </c>
       <c r="J277" s="1">
         <v>10</v>
@@ -13325,7 +13325,7 @@
       </c>
       <c r="I278" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>736544236</v>
+        <v>331784785</v>
       </c>
       <c r="J278" s="1">
         <v>10</v>
@@ -13367,7 +13367,7 @@
       </c>
       <c r="I279" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>881947842</v>
+        <v>546042410</v>
       </c>
       <c r="J279" s="1">
         <v>10</v>
@@ -13415,7 +13415,7 @@
       </c>
       <c r="I280" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>177279991</v>
+        <v>407353211</v>
       </c>
       <c r="J280" s="1">
         <v>10</v>
@@ -13457,7 +13457,7 @@
       </c>
       <c r="I281" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>89016104</v>
+        <v>370442173</v>
       </c>
       <c r="J281" s="1">
         <v>10</v>
@@ -13499,7 +13499,7 @@
       </c>
       <c r="I282" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>816680359</v>
+        <v>565239947</v>
       </c>
       <c r="J282" s="1">
         <v>10</v>
@@ -13541,7 +13541,7 @@
       </c>
       <c r="I283" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>757218451</v>
+        <v>222633151</v>
       </c>
       <c r="J283" s="1">
         <v>10</v>
@@ -13583,7 +13583,7 @@
       </c>
       <c r="I284" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>370205935</v>
+        <v>897810614</v>
       </c>
       <c r="J284" s="1">
         <v>10</v>
@@ -13628,7 +13628,7 @@
       </c>
       <c r="I285" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>501346915</v>
+        <v>321890199</v>
       </c>
       <c r="J285" s="1">
         <v>10</v>
@@ -13670,7 +13670,7 @@
       </c>
       <c r="I286" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>255171199</v>
+        <v>399862117</v>
       </c>
       <c r="J286" s="1">
         <v>10</v>
@@ -13712,7 +13712,7 @@
       </c>
       <c r="I287" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>122575515</v>
+        <v>554498970</v>
       </c>
       <c r="J287" s="1">
         <v>10</v>
@@ -13754,7 +13754,7 @@
       </c>
       <c r="I288" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>655988308</v>
+        <v>644040407</v>
       </c>
       <c r="J288" s="1">
         <v>10</v>
@@ -13796,7 +13796,7 @@
       </c>
       <c r="I289" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>181356805</v>
+        <v>15782539</v>
       </c>
       <c r="J289" s="1">
         <v>10</v>
@@ -13838,7 +13838,7 @@
       </c>
       <c r="I290" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>821932828</v>
+        <v>657780595</v>
       </c>
       <c r="J290" s="1">
         <v>10</v>
@@ -13883,7 +13883,7 @@
       </c>
       <c r="I291" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>808163543</v>
+        <v>941480984</v>
       </c>
       <c r="J291" s="1">
         <v>10</v>
@@ -13925,7 +13925,7 @@
       </c>
       <c r="I292" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>694768513</v>
+        <v>259708027</v>
       </c>
       <c r="J292" s="1">
         <v>10</v>
@@ -13967,7 +13967,7 @@
       </c>
       <c r="I293" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>832040136</v>
+        <v>68655485</v>
       </c>
       <c r="J293" s="1">
         <v>10</v>
@@ -14009,7 +14009,7 @@
       </c>
       <c r="I294" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>374171986</v>
+        <v>72707559</v>
       </c>
       <c r="J294" s="1">
         <v>10</v>
@@ -14054,7 +14054,7 @@
       </c>
       <c r="I295" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>385358428</v>
+        <v>610112429</v>
       </c>
       <c r="J295" s="1">
         <v>10</v>
@@ -14096,7 +14096,7 @@
       </c>
       <c r="I296" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>421717478</v>
+        <v>534266214</v>
       </c>
       <c r="J296" s="1">
         <v>10</v>
@@ -14138,7 +14138,7 @@
       </c>
       <c r="I297" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>416734422</v>
+        <v>696430513</v>
       </c>
       <c r="J297" s="1">
         <v>10</v>
@@ -14180,7 +14180,7 @@
       </c>
       <c r="I298" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>950330200</v>
+        <v>433117417</v>
       </c>
       <c r="J298" s="1">
         <v>10</v>
@@ -14222,7 +14222,7 @@
       </c>
       <c r="I299" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>742720305</v>
+        <v>649662578</v>
       </c>
       <c r="J299" s="1">
         <v>10</v>
@@ -14270,7 +14270,7 @@
       </c>
       <c r="I300" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>208662119</v>
+        <v>190282525</v>
       </c>
       <c r="J300" s="1">
         <v>10</v>
@@ -14312,7 +14312,7 @@
       </c>
       <c r="I301" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>345333687</v>
+        <v>466950813</v>
       </c>
       <c r="J301" s="1">
         <v>10</v>
@@ -14354,7 +14354,7 @@
       </c>
       <c r="I302" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>399104721</v>
+        <v>304953300</v>
       </c>
       <c r="J302" s="1">
         <v>10</v>
@@ -14396,7 +14396,7 @@
       </c>
       <c r="I303" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>21520151</v>
+        <v>207372828</v>
       </c>
       <c r="J303" s="1">
         <v>10</v>
@@ -14438,7 +14438,7 @@
       </c>
       <c r="I304" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>492181016</v>
+        <v>577293195</v>
       </c>
       <c r="J304" s="1">
         <v>10</v>
@@ -14483,7 +14483,7 @@
       </c>
       <c r="I305" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>934958758</v>
+        <v>582738502</v>
       </c>
       <c r="J305" s="1">
         <v>10</v>
@@ -14525,7 +14525,7 @@
       </c>
       <c r="I306" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>231369784</v>
+        <v>348954075</v>
       </c>
       <c r="J306" s="1">
         <v>10</v>
@@ -14567,7 +14567,7 @@
       </c>
       <c r="I307" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>220107658</v>
+        <v>162625612</v>
       </c>
       <c r="J307" s="1">
         <v>10</v>
@@ -14609,7 +14609,7 @@
       </c>
       <c r="I308" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>199590044</v>
+        <v>341708289</v>
       </c>
       <c r="J308" s="1">
         <v>10</v>
@@ -14651,7 +14651,7 @@
       </c>
       <c r="I309" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>21257256</v>
+        <v>540834905</v>
       </c>
       <c r="J309" s="1">
         <v>10</v>
@@ -14693,7 +14693,7 @@
       </c>
       <c r="I310" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>617892591</v>
+        <v>642046408</v>
       </c>
       <c r="J310" s="1">
         <v>10</v>
@@ -14738,7 +14738,7 @@
       </c>
       <c r="I311" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>789693706</v>
+        <v>546287164</v>
       </c>
       <c r="J311" s="1">
         <v>10</v>
@@ -14780,7 +14780,7 @@
       </c>
       <c r="I312" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>860490152</v>
+        <v>513960364</v>
       </c>
       <c r="J312" s="1">
         <v>10</v>
@@ -14822,7 +14822,7 @@
       </c>
       <c r="I313" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>666821786</v>
+        <v>978923035</v>
       </c>
       <c r="J313" s="1">
         <v>10</v>
@@ -14864,7 +14864,7 @@
       </c>
       <c r="I314" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>75068164</v>
+        <v>704652755</v>
       </c>
       <c r="J314" s="1">
         <v>10</v>
@@ -14909,7 +14909,7 @@
       </c>
       <c r="I315" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>367963732</v>
+        <v>575782622</v>
       </c>
       <c r="J315" s="1">
         <v>10</v>
@@ -14951,7 +14951,7 @@
       </c>
       <c r="I316" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>946174340</v>
+        <v>127659036</v>
       </c>
       <c r="J316" s="1">
         <v>10</v>
@@ -14993,7 +14993,7 @@
       </c>
       <c r="I317" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>814208410</v>
+        <v>198780540</v>
       </c>
       <c r="J317" s="1">
         <v>10</v>
@@ -15035,7 +15035,7 @@
       </c>
       <c r="I318" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>729640689</v>
+        <v>575985768</v>
       </c>
       <c r="J318" s="1">
         <v>10</v>
@@ -15077,7 +15077,7 @@
       </c>
       <c r="I319" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>486174688</v>
+        <v>840586320</v>
       </c>
       <c r="J319" s="1">
         <v>10</v>
@@ -15125,7 +15125,7 @@
       </c>
       <c r="I320" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>477431772</v>
+        <v>973686642</v>
       </c>
       <c r="J320" s="1">
         <v>10</v>
@@ -15167,7 +15167,7 @@
       </c>
       <c r="I321" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>470379281</v>
+        <v>963209024</v>
       </c>
       <c r="J321" s="1">
         <v>10</v>
@@ -15209,7 +15209,7 @@
       </c>
       <c r="I322" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>625215449</v>
+        <v>835732079</v>
       </c>
       <c r="J322" s="1">
         <v>10</v>
@@ -15251,7 +15251,7 @@
       </c>
       <c r="I323" s="1">
         <f t="shared" ref="I323:I363" ca="1" si="5">RANDBETWEEN(10000, 999999999)</f>
-        <v>682313177</v>
+        <v>922120690</v>
       </c>
       <c r="J323" s="1">
         <v>10</v>
@@ -15293,7 +15293,7 @@
       </c>
       <c r="I324" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>916714897</v>
+        <v>704029781</v>
       </c>
       <c r="J324" s="1">
         <v>10</v>
@@ -15338,7 +15338,7 @@
       </c>
       <c r="I325" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>25896278</v>
+        <v>861396197</v>
       </c>
       <c r="J325" s="1">
         <v>10</v>
@@ -15380,7 +15380,7 @@
       </c>
       <c r="I326" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>464543119</v>
+        <v>937249013</v>
       </c>
       <c r="J326" s="1">
         <v>10</v>
@@ -15422,7 +15422,7 @@
       </c>
       <c r="I327" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>929699035</v>
+        <v>442062931</v>
       </c>
       <c r="J327" s="1">
         <v>10</v>
@@ -15464,7 +15464,7 @@
       </c>
       <c r="I328" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>285124538</v>
+        <v>927171062</v>
       </c>
       <c r="J328" s="1">
         <v>10</v>
@@ -15506,7 +15506,7 @@
       </c>
       <c r="I329" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>364817590</v>
+        <v>708917117</v>
       </c>
       <c r="J329" s="1">
         <v>10</v>
@@ -15548,7 +15548,7 @@
       </c>
       <c r="I330" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>103026068</v>
+        <v>414801710</v>
       </c>
       <c r="J330" s="1">
         <v>10</v>
@@ -15593,7 +15593,7 @@
       </c>
       <c r="I331" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>95939729</v>
+        <v>649128891</v>
       </c>
       <c r="J331" s="1">
         <v>10</v>
@@ -15635,7 +15635,7 @@
       </c>
       <c r="I332" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>158036732</v>
+        <v>223144994</v>
       </c>
       <c r="J332" s="1">
         <v>10</v>
@@ -15677,7 +15677,7 @@
       </c>
       <c r="I333" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>248486350</v>
+        <v>777204373</v>
       </c>
       <c r="J333" s="1">
         <v>10</v>
@@ -15719,7 +15719,7 @@
       </c>
       <c r="I334" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>158373115</v>
+        <v>546093826</v>
       </c>
       <c r="J334" s="1">
         <v>10</v>
@@ -15764,7 +15764,7 @@
       </c>
       <c r="I335" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>319632477</v>
+        <v>128858133</v>
       </c>
       <c r="J335" s="1">
         <v>10</v>
@@ -15806,7 +15806,7 @@
       </c>
       <c r="I336" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>561068625</v>
+        <v>421795997</v>
       </c>
       <c r="J336" s="1">
         <v>10</v>
@@ -15848,7 +15848,7 @@
       </c>
       <c r="I337" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>342970281</v>
+        <v>53539403</v>
       </c>
       <c r="J337" s="1">
         <v>10</v>
@@ -15890,7 +15890,7 @@
       </c>
       <c r="I338" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>869392670</v>
+        <v>578071647</v>
       </c>
       <c r="J338" s="1">
         <v>10</v>
@@ -15932,7 +15932,7 @@
       </c>
       <c r="I339" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>901172661</v>
+        <v>671717681</v>
       </c>
       <c r="J339" s="1">
         <v>10</v>
@@ -15980,7 +15980,7 @@
       </c>
       <c r="I340" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>423906122</v>
+        <v>160926835</v>
       </c>
       <c r="J340" s="1">
         <v>10</v>
@@ -16022,7 +16022,7 @@
       </c>
       <c r="I341" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>628110973</v>
+        <v>712142454</v>
       </c>
       <c r="J341" s="1">
         <v>10</v>
@@ -16064,7 +16064,7 @@
       </c>
       <c r="I342" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>476490163</v>
+        <v>239353256</v>
       </c>
       <c r="J342" s="1">
         <v>10</v>
@@ -16106,7 +16106,7 @@
       </c>
       <c r="I343" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>895476591</v>
+        <v>274099468</v>
       </c>
       <c r="J343" s="1">
         <v>10</v>
@@ -16148,7 +16148,7 @@
       </c>
       <c r="I344" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>886373723</v>
+        <v>342062439</v>
       </c>
       <c r="J344" s="1">
         <v>10</v>
@@ -16193,7 +16193,7 @@
       </c>
       <c r="I345" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>305805779</v>
+        <v>689747997</v>
       </c>
       <c r="J345" s="1">
         <v>10</v>
@@ -16235,7 +16235,7 @@
       </c>
       <c r="I346" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>922275693</v>
+        <v>848398533</v>
       </c>
       <c r="J346" s="1">
         <v>10</v>
@@ -16277,7 +16277,7 @@
       </c>
       <c r="I347" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>568081144</v>
+        <v>965321087</v>
       </c>
       <c r="J347" s="1">
         <v>10</v>
@@ -16319,7 +16319,7 @@
       </c>
       <c r="I348" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>380195437</v>
+        <v>63464899</v>
       </c>
       <c r="J348" s="1">
         <v>10</v>
@@ -16361,7 +16361,7 @@
       </c>
       <c r="I349" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>587309734</v>
+        <v>482469077</v>
       </c>
       <c r="J349" s="1">
         <v>10</v>
@@ -16403,7 +16403,7 @@
       </c>
       <c r="I350" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>607349213</v>
+        <v>986384880</v>
       </c>
       <c r="J350" s="1">
         <v>10</v>
@@ -16448,7 +16448,7 @@
       </c>
       <c r="I351" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>634768098</v>
+        <v>267682009</v>
       </c>
       <c r="J351" s="1">
         <v>10</v>
@@ -16490,7 +16490,7 @@
       </c>
       <c r="I352" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>17135810</v>
+        <v>597701111</v>
       </c>
       <c r="J352" s="1">
         <v>10</v>
@@ -16532,7 +16532,7 @@
       </c>
       <c r="I353" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>943961105</v>
+        <v>659043862</v>
       </c>
       <c r="J353" s="1">
         <v>10</v>
@@ -16574,7 +16574,7 @@
       </c>
       <c r="I354" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>864310363</v>
+        <v>661834386</v>
       </c>
       <c r="J354" s="1">
         <v>10</v>
@@ -16619,7 +16619,7 @@
       </c>
       <c r="I355" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>544784127</v>
+        <v>521038791</v>
       </c>
       <c r="J355" s="1">
         <v>10</v>
@@ -16661,7 +16661,7 @@
       </c>
       <c r="I356" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>670314309</v>
+        <v>536246833</v>
       </c>
       <c r="J356" s="1">
         <v>10</v>
@@ -16703,7 +16703,7 @@
       </c>
       <c r="I357" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>428395368</v>
+        <v>848008493</v>
       </c>
       <c r="J357" s="1">
         <v>10</v>
@@ -16745,7 +16745,7 @@
       </c>
       <c r="I358" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>892050025</v>
+        <v>67155249</v>
       </c>
       <c r="J358" s="1">
         <v>10</v>
@@ -16787,7 +16787,7 @@
       </c>
       <c r="I359" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>169939295</v>
+        <v>346733910</v>
       </c>
       <c r="J359" s="1">
         <v>10</v>
@@ -16835,7 +16835,7 @@
       </c>
       <c r="I360" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>815949204</v>
+        <v>609109093</v>
       </c>
       <c r="J360" s="1">
         <v>10</v>
@@ -16877,7 +16877,7 @@
       </c>
       <c r="I361" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>747439353</v>
+        <v>450669304</v>
       </c>
       <c r="J361" s="1">
         <v>10</v>
@@ -16919,7 +16919,7 @@
       </c>
       <c r="I362" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>707841905</v>
+        <v>221142600</v>
       </c>
       <c r="J362" s="1">
         <v>10</v>
@@ -16961,7 +16961,7 @@
       </c>
       <c r="I363" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>88693525</v>
+        <v>495260996</v>
       </c>
       <c r="J363" s="1">
         <v>10</v>

</xml_diff>